<commit_message>
Updated the P core dimensions
</commit_message>
<xml_diff>
--- a/Cores-Info-Database.xlsx
+++ b/Cores-Info-Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19725\Desktop\education\college\extracurriculars\pemg research\PEMG_Design_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{69337D6E-0B5F-4307-8992-FC53D8569CA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B381F49-E9EF-4BCE-A2CD-C1384D22E827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{FD5E7F2C-425F-4B8A-9B1F-7669120DD1D5}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="497">
   <si>
     <t>E 5</t>
   </si>
@@ -1216,123 +1216,27 @@
     <t>P 9 x. 5 (center)</t>
   </si>
   <si>
-    <t>12.5 / 13.4 mm</t>
-  </si>
-  <si>
-    <t>10/11.9 mm^2</t>
-  </si>
-  <si>
-    <t>0/9.3 mm^2</t>
-  </si>
-  <si>
-    <t>125/159 mm^3</t>
-  </si>
-  <si>
     <t>P 11 x 7 (center)</t>
   </si>
   <si>
-    <t>15.9 / 16.3 mm</t>
-  </si>
-  <si>
-    <t>15.9 / 17.7mm^2</t>
-  </si>
-  <si>
-    <t>0/14.1 mm^2</t>
-  </si>
-  <si>
-    <t>253/289 mm^3</t>
-  </si>
-  <si>
     <t>P 14 x 8 (center)</t>
   </si>
   <si>
-    <t>20/21 mm</t>
-  </si>
-  <si>
-    <t>25/28.7 mm^2</t>
-  </si>
-  <si>
-    <t>20/23.6 mm^2</t>
-  </si>
-  <si>
-    <t>500/603 mm^3</t>
-  </si>
-  <si>
     <t>P 18 x 11(center)</t>
   </si>
   <si>
-    <t>25.9/26.6 mm</t>
-  </si>
-  <si>
-    <t>43/46.7 mm^2</t>
-  </si>
-  <si>
-    <t>0/33.9 mm^2</t>
-  </si>
-  <si>
-    <t>1114/1242 mm^3</t>
-  </si>
-  <si>
     <t>P 22 x 13(center)</t>
   </si>
   <si>
-    <t>31.6 / 33.2 mm</t>
-  </si>
-  <si>
-    <t>63/72.6 mm^2</t>
-  </si>
-  <si>
-    <t>0/58.1 mm^2</t>
-  </si>
-  <si>
-    <t>1990/2410</t>
-  </si>
-  <si>
     <t>P 26 x 16 (center)</t>
   </si>
   <si>
-    <t>37.2/40 mm</t>
-  </si>
-  <si>
-    <t>93/108 mm^2</t>
-  </si>
-  <si>
-    <t>76.5/87 mm^2</t>
-  </si>
-  <si>
-    <t>3460/4320 mm^3</t>
-  </si>
-  <si>
     <t>P 30 x 19 (center)</t>
   </si>
   <si>
-    <t>45/46 mm</t>
-  </si>
-  <si>
-    <t>136/145 mm^2</t>
-  </si>
-  <si>
-    <t>0/117 mm^2</t>
-  </si>
-  <si>
-    <t>6120/6670 mm^3</t>
-  </si>
-  <si>
     <t>P 36 x 22 (center)</t>
   </si>
   <si>
-    <t>52/53.5 mm</t>
-  </si>
-  <si>
-    <t>202/213 mm^2</t>
-  </si>
-  <si>
-    <t>0/173 mm^2</t>
-  </si>
-  <si>
-    <t>10500/11400 mm^3</t>
-  </si>
-  <si>
     <t>P 41 x 25</t>
   </si>
   <si>
@@ -1529,6 +1433,84 @@
   </si>
   <si>
     <t>Core factor</t>
+  </si>
+  <si>
+    <t>12.5 mm</t>
+  </si>
+  <si>
+    <t>15.9 mm</t>
+  </si>
+  <si>
+    <t>20 mm</t>
+  </si>
+  <si>
+    <t>25.9 mm</t>
+  </si>
+  <si>
+    <t>31.6 mm</t>
+  </si>
+  <si>
+    <t>45 mm</t>
+  </si>
+  <si>
+    <t>52 mm</t>
+  </si>
+  <si>
+    <t>10 mm^2</t>
+  </si>
+  <si>
+    <t>15.9 mm^2</t>
+  </si>
+  <si>
+    <t>25 mm^2</t>
+  </si>
+  <si>
+    <t>43 mm^2</t>
+  </si>
+  <si>
+    <t>63 mm^2</t>
+  </si>
+  <si>
+    <t>93 mm^2</t>
+  </si>
+  <si>
+    <t>136 mm^2</t>
+  </si>
+  <si>
+    <t>202 mm^2</t>
+  </si>
+  <si>
+    <t>0 mm^2</t>
+  </si>
+  <si>
+    <t>20 mm^2</t>
+  </si>
+  <si>
+    <t>76.5 mm^2</t>
+  </si>
+  <si>
+    <t>125 mm^3</t>
+  </si>
+  <si>
+    <t>253 mm^3</t>
+  </si>
+  <si>
+    <t>500 mm^3</t>
+  </si>
+  <si>
+    <t>1114 mm^3</t>
+  </si>
+  <si>
+    <t>1990 mm^3</t>
+  </si>
+  <si>
+    <t>3460 mm^3</t>
+  </si>
+  <si>
+    <t>6120 mm^3</t>
+  </si>
+  <si>
+    <t>10500 mm^3</t>
   </si>
 </sst>
 </file>
@@ -2052,7 +2034,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2432,8 +2414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50AB67D-9472-4E0F-AB22-86EA84CCBB8E}">
   <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="J98" sqref="J98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2451,31 +2433,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>492</v>
+        <v>460</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>493</v>
+        <v>461</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>494</v>
+        <v>462</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>495</v>
+        <v>463</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>496</v>
+        <v>464</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>497</v>
+        <v>465</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>498</v>
+        <v>466</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>501</v>
+        <v>469</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>502</v>
+        <v>470</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2896,7 +2878,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>104</v>
       </c>
@@ -2915,7 +2897,7 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>109</v>
       </c>
@@ -2934,7 +2916,7 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>114</v>
       </c>
@@ -2953,7 +2935,7 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>115</v>
       </c>
@@ -2972,7 +2954,7 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>119</v>
       </c>
@@ -2991,7 +2973,7 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>121</v>
       </c>
@@ -3010,7 +2992,7 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
         <v>126</v>
       </c>
@@ -3029,7 +3011,7 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>127</v>
       </c>
@@ -3048,7 +3030,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>132</v>
       </c>
@@ -3067,7 +3049,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
         <v>135</v>
       </c>
@@ -3086,7 +3068,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
         <v>136</v>
       </c>
@@ -3105,7 +3087,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
         <v>141</v>
       </c>
@@ -3124,7 +3106,7 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>146</v>
       </c>
@@ -3143,7 +3125,7 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>148</v>
       </c>
@@ -3162,7 +3144,7 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>153</v>
       </c>
@@ -3181,7 +3163,7 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
         <v>155</v>
       </c>
@@ -3200,7 +3182,7 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
         <v>160</v>
       </c>
@@ -3219,7 +3201,7 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
         <v>161</v>
       </c>
@@ -3238,7 +3220,7 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
         <v>166</v>
       </c>
@@ -3257,7 +3239,7 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
         <v>171</v>
       </c>
@@ -3276,7 +3258,7 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
         <v>175</v>
       </c>
@@ -3295,7 +3277,7 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
         <v>179</v>
       </c>
@@ -3314,7 +3296,7 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
         <v>184</v>
       </c>
@@ -3333,7 +3315,7 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
         <v>188</v>
       </c>
@@ -3352,7 +3334,7 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
         <v>193</v>
       </c>
@@ -3371,7 +3353,7 @@
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
         <v>198</v>
       </c>
@@ -3390,7 +3372,7 @@
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
-    <row r="50" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
         <v>203</v>
       </c>
@@ -3409,7 +3391,7 @@
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
         <v>208</v>
       </c>
@@ -3428,7 +3410,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
         <v>213</v>
       </c>
@@ -3447,7 +3429,7 @@
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="1" t="s">
         <v>218</v>
       </c>
@@ -3466,7 +3448,7 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="1" t="s">
         <v>223</v>
       </c>
@@ -3485,7 +3467,7 @@
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
     </row>
-    <row r="55" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
         <v>228</v>
       </c>
@@ -3504,7 +3486,7 @@
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
     </row>
-    <row r="56" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="1" t="s">
         <v>233</v>
       </c>
@@ -3523,7 +3505,7 @@
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
     </row>
-    <row r="57" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="1" t="s">
         <v>238</v>
       </c>
@@ -3542,7 +3524,7 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
     </row>
-    <row r="58" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="1" t="s">
         <v>242</v>
       </c>
@@ -3561,7 +3543,7 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
     </row>
-    <row r="59" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="1" t="s">
         <v>246</v>
       </c>
@@ -3580,7 +3562,7 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
     </row>
-    <row r="60" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="1" t="s">
         <v>251</v>
       </c>
@@ -3599,7 +3581,7 @@
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
     </row>
-    <row r="61" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="1" t="s">
         <v>256</v>
       </c>
@@ -3618,7 +3600,7 @@
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="1" t="s">
         <v>258</v>
       </c>
@@ -3637,7 +3619,7 @@
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
     </row>
-    <row r="63" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="1" t="s">
         <v>263</v>
       </c>
@@ -3656,7 +3638,7 @@
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
     </row>
-    <row r="64" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="1" t="s">
         <v>264</v>
       </c>
@@ -3675,7 +3657,7 @@
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
     </row>
-    <row r="65" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="1" t="s">
         <v>269</v>
       </c>
@@ -3694,7 +3676,7 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
     </row>
-    <row r="66" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="1" t="s">
         <v>274</v>
       </c>
@@ -3713,7 +3695,7 @@
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
     </row>
-    <row r="67" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" s="1" t="s">
         <v>279</v>
       </c>
@@ -3732,7 +3714,7 @@
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
     </row>
-    <row r="68" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="1" t="s">
         <v>283</v>
       </c>
@@ -3751,7 +3733,7 @@
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
     </row>
-    <row r="69" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="1" t="s">
         <v>286</v>
       </c>
@@ -3770,7 +3752,7 @@
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
     </row>
-    <row r="70" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="1" t="s">
         <v>289</v>
       </c>
@@ -3789,7 +3771,7 @@
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
     </row>
-    <row r="71" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="1" t="s">
         <v>294</v>
       </c>
@@ -3808,7 +3790,7 @@
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
     </row>
-    <row r="72" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A72" s="1" t="s">
         <v>298</v>
       </c>
@@ -3827,7 +3809,7 @@
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
     </row>
-    <row r="73" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="1" t="s">
         <v>299</v>
       </c>
@@ -3846,7 +3828,7 @@
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
     </row>
-    <row r="74" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="1" t="s">
         <v>304</v>
       </c>
@@ -3865,7 +3847,7 @@
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
     </row>
-    <row r="75" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="1" t="s">
         <v>305</v>
       </c>
@@ -3884,7 +3866,7 @@
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
     </row>
-    <row r="76" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="1" t="s">
         <v>310</v>
       </c>
@@ -3903,7 +3885,7 @@
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
     </row>
-    <row r="77" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="1" t="s">
         <v>312</v>
       </c>
@@ -3922,7 +3904,7 @@
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
     </row>
-    <row r="78" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="1" t="s">
         <v>316</v>
       </c>
@@ -3941,7 +3923,7 @@
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
     </row>
-    <row r="79" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="1" t="s">
         <v>321</v>
       </c>
@@ -3962,7 +3944,7 @@
     </row>
     <row r="80" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
-        <v>500</v>
+        <v>468</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>295</v>
@@ -3979,7 +3961,7 @@
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
     </row>
-    <row r="81" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="1" t="s">
         <v>329</v>
       </c>
@@ -3998,7 +3980,7 @@
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
     </row>
-    <row r="82" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="1" t="s">
         <v>334</v>
       </c>
@@ -4017,7 +3999,7 @@
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
     </row>
-    <row r="83" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" s="1" t="s">
         <v>339</v>
       </c>
@@ -4036,7 +4018,7 @@
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
     </row>
-    <row r="84" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="1" t="s">
         <v>344</v>
       </c>
@@ -4057,7 +4039,7 @@
     </row>
     <row r="85" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
-        <v>499</v>
+        <v>467</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>348</v>
@@ -4074,7 +4056,7 @@
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
     </row>
-    <row r="86" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="1" t="s">
         <v>352</v>
       </c>
@@ -4093,7 +4075,7 @@
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
     </row>
-    <row r="87" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="1" t="s">
         <v>356</v>
       </c>
@@ -4112,7 +4094,7 @@
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
     </row>
-    <row r="88" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="1" t="s">
         <v>361</v>
       </c>
@@ -4131,7 +4113,7 @@
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
     </row>
-    <row r="89" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" s="1" t="s">
         <v>366</v>
       </c>
@@ -4150,7 +4132,7 @@
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
     </row>
-    <row r="90" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A90" s="1" t="s">
         <v>371</v>
       </c>
@@ -4169,7 +4151,7 @@
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
     </row>
-    <row r="91" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" s="1" t="s">
         <v>376</v>
       </c>
@@ -4188,7 +4170,7 @@
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
     </row>
-    <row r="92" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A92" s="1" t="s">
         <v>381</v>
       </c>
@@ -4205,7 +4187,7 @@
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
     </row>
-    <row r="93" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="1" t="s">
         <v>385</v>
       </c>
@@ -4222,7 +4204,7 @@
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
     </row>
-    <row r="94" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="1" t="s">
         <v>389</v>
       </c>
@@ -4256,164 +4238,164 @@
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
     </row>
-    <row r="96" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" s="1" t="s">
         <v>397</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>398</v>
+        <v>471</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>399</v>
+        <v>478</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>400</v>
+        <v>486</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>401</v>
+        <v>489</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
     </row>
-    <row r="97" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>403</v>
+        <v>472</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>404</v>
+        <v>479</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>405</v>
+        <v>486</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>406</v>
+        <v>490</v>
       </c>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
     </row>
-    <row r="98" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="1" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>408</v>
+        <v>473</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>409</v>
+        <v>480</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>410</v>
+        <v>487</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>411</v>
+        <v>491</v>
       </c>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
     </row>
-    <row r="99" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="1" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>413</v>
+        <v>474</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>414</v>
+        <v>481</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>415</v>
+        <v>486</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>416</v>
+        <v>492</v>
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
     </row>
-    <row r="100" spans="1:7" ht="39" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" s="1" t="s">
-        <v>417</v>
+        <v>401</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>418</v>
+        <v>475</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>419</v>
+        <v>482</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>420</v>
+        <v>486</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>421</v>
+        <v>493</v>
       </c>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
     </row>
-    <row r="101" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="1" t="s">
-        <v>422</v>
+        <v>402</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>424</v>
+        <v>483</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>425</v>
+        <v>488</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>426</v>
+        <v>494</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
     </row>
-    <row r="102" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="1" t="s">
-        <v>427</v>
+        <v>403</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>428</v>
+        <v>476</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>429</v>
+        <v>484</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>430</v>
+        <v>486</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>431</v>
+        <v>495</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
     </row>
-    <row r="103" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" s="1" t="s">
-        <v>432</v>
+        <v>404</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>433</v>
+        <v>477</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>434</v>
+        <v>485</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>435</v>
+        <v>486</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>436</v>
+        <v>496</v>
       </c>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
     </row>
-    <row r="104" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="1" t="s">
-        <v>437</v>
+        <v>405</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>438</v>
+        <v>406</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>117</v>
@@ -4422,216 +4404,216 @@
         <v>354</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>439</v>
+        <v>407</v>
       </c>
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
     </row>
-    <row r="105" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="1" t="s">
-        <v>440</v>
+        <v>408</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>441</v>
+        <v>409</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>220</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>442</v>
+        <v>410</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>443</v>
+        <v>411</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
     </row>
-    <row r="106" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="1" t="s">
-        <v>444</v>
+        <v>412</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>445</v>
+        <v>413</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>446</v>
+        <v>414</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>447</v>
+        <v>415</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>448</v>
+        <v>416</v>
       </c>
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
     </row>
-    <row r="107" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A107" s="1" t="s">
-        <v>449</v>
+        <v>417</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>450</v>
+        <v>418</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>451</v>
+        <v>419</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>452</v>
+        <v>420</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>453</v>
+        <v>421</v>
       </c>
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
     </row>
-    <row r="108" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A108" s="1" t="s">
-        <v>454</v>
+        <v>422</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>455</v>
+        <v>423</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>456</v>
+        <v>424</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>457</v>
+        <v>425</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>458</v>
+        <v>426</v>
       </c>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
     </row>
-    <row r="109" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A109" s="1" t="s">
-        <v>459</v>
+        <v>427</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>460</v>
+        <v>428</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>461</v>
+        <v>429</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>462</v>
+        <v>430</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>463</v>
+        <v>431</v>
       </c>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
     </row>
-    <row r="110" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A110" s="1" t="s">
-        <v>464</v>
+        <v>432</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>465</v>
+        <v>433</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>466</v>
+        <v>434</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>462</v>
+        <v>430</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>467</v>
+        <v>435</v>
       </c>
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
     </row>
-    <row r="111" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A111" s="1" t="s">
-        <v>468</v>
+        <v>436</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>469</v>
+        <v>437</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>470</v>
+        <v>438</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>471</v>
+        <v>439</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>472</v>
+        <v>440</v>
       </c>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
     </row>
-    <row r="112" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="1" t="s">
-        <v>473</v>
+        <v>441</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>474</v>
+        <v>442</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>475</v>
+        <v>443</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>471</v>
+        <v>439</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>476</v>
+        <v>444</v>
       </c>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
     </row>
-    <row r="113" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A113" s="1" t="s">
-        <v>477</v>
+        <v>445</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>478</v>
+        <v>446</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>479</v>
+        <v>447</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>480</v>
+        <v>448</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>481</v>
+        <v>449</v>
       </c>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
     </row>
-    <row r="114" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A114" s="1" t="s">
-        <v>482</v>
+        <v>450</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>483</v>
+        <v>451</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>484</v>
+        <v>452</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>485</v>
+        <v>453</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>486</v>
+        <v>454</v>
       </c>
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
     </row>
-    <row r="115" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A115" s="1" t="s">
-        <v>487</v>
+        <v>455</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>488</v>
+        <v>456</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>489</v>
+        <v>457</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>490</v>
+        <v>458</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>491</v>
+        <v>459</v>
       </c>
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>

</xml_diff>

<commit_message>
Removed an unecessary label
</commit_message>
<xml_diff>
--- a/Cores-Info-Database.xlsx
+++ b/Cores-Info-Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19725\Desktop\education\college\extracurriculars\pemg research\PEMG_Design_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B381F49-E9EF-4BCE-A2CD-C1384D22E827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{971529F9-A283-4545-9B81-799292167CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{FD5E7F2C-425F-4B8A-9B1F-7669120DD1D5}"/>
   </bookViews>
@@ -1213,30 +1213,6 @@
     <t>70 mm^3</t>
   </si>
   <si>
-    <t>P 9 x. 5 (center)</t>
-  </si>
-  <si>
-    <t>P 11 x 7 (center)</t>
-  </si>
-  <si>
-    <t>P 14 x 8 (center)</t>
-  </si>
-  <si>
-    <t>P 18 x 11(center)</t>
-  </si>
-  <si>
-    <t>P 22 x 13(center)</t>
-  </si>
-  <si>
-    <t>P 26 x 16 (center)</t>
-  </si>
-  <si>
-    <t>P 30 x 19 (center)</t>
-  </si>
-  <si>
-    <t>P 36 x 22 (center)</t>
-  </si>
-  <si>
     <t>P 41 x 25</t>
   </si>
   <si>
@@ -1511,6 +1487,30 @@
   </si>
   <si>
     <t>10500 mm^3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P 9 x. 5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P 11 x 7 </t>
+  </si>
+  <si>
+    <t>P 14 x 8</t>
+  </si>
+  <si>
+    <t>P 18 x 11</t>
+  </si>
+  <si>
+    <t>P 22 x 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P 26 x 16 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">P 30 x 19 </t>
+  </si>
+  <si>
+    <t>P 36 x 22</t>
   </si>
 </sst>
 </file>
@@ -2415,7 +2415,7 @@
   <dimension ref="A1:I117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="J98" sqref="J98"/>
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2433,31 +2433,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>462</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>469</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3944,7 +3944,7 @@
     </row>
     <row r="80" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="1" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>295</v>
@@ -4039,7 +4039,7 @@
     </row>
     <row r="85" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="1" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>348</v>
@@ -4240,162 +4240,162 @@
     </row>
     <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" s="1" t="s">
-        <v>397</v>
+        <v>489</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="C96" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D96" s="1" t="s">
         <v>478</v>
       </c>
-      <c r="D96" s="1" t="s">
-        <v>486</v>
-      </c>
       <c r="E96" s="1" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
     </row>
     <row r="97" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="1" t="s">
-        <v>398</v>
+        <v>490</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
     </row>
     <row r="98" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="1" t="s">
-        <v>399</v>
+        <v>491</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
     </row>
     <row r="99" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="1" t="s">
-        <v>400</v>
+        <v>492</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
     </row>
     <row r="100" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" s="1" t="s">
-        <v>401</v>
+        <v>493</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
     </row>
     <row r="101" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="1" t="s">
-        <v>402</v>
+        <v>494</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
     </row>
     <row r="102" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="1" t="s">
-        <v>403</v>
+        <v>495</v>
       </c>
       <c r="B102" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="C102" s="1" t="s">
         <v>476</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>484</v>
-      </c>
       <c r="D102" s="1" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
     </row>
     <row r="103" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" s="1" t="s">
-        <v>404</v>
+        <v>496</v>
       </c>
       <c r="B103" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>477</v>
       </c>
-      <c r="C103" s="1" t="s">
-        <v>485</v>
-      </c>
       <c r="D103" s="1" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
     </row>
     <row r="104" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="1" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>117</v>
@@ -4404,216 +4404,216 @@
         <v>354</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
     </row>
     <row r="105" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="1" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>220</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
     </row>
     <row r="106" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="1" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
     </row>
     <row r="107" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A107" s="1" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
     </row>
     <row r="108" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A108" s="1" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
     </row>
     <row r="109" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A109" s="1" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
     </row>
     <row r="110" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A110" s="1" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
     </row>
     <row r="111" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A111" s="1" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
     </row>
     <row r="112" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="1" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
     </row>
     <row r="113" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A113" s="1" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
     </row>
     <row r="114" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A114" s="1" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
     </row>
     <row r="115" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A115" s="1" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>

</xml_diff>

<commit_message>
Finished the bobbin window area and core window area columns
</commit_message>
<xml_diff>
--- a/Cores-Info-Database.xlsx
+++ b/Cores-Info-Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19725\Desktop\education\college\extracurriculars\pemg research\PEMG_Design_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0277A5-781D-4AE0-AC13-AE9E49CE257B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E17DD71-7354-467E-AD78-6B7758038915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{FD5E7F2C-425F-4B8A-9B1F-7669120DD1D5}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="125">
   <si>
     <t>E 5</t>
   </si>
@@ -392,6 +392,9 @@
   </si>
   <si>
     <t xml:space="preserve">P 9 x 5 </t>
+  </si>
+  <si>
+    <t>l_N</t>
   </si>
 </sst>
 </file>
@@ -922,7 +925,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -939,13 +942,10 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1329,18 +1329,18 @@
   <dimension ref="A1:I117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.6328125" customWidth="1"/>
-    <col min="2" max="2" width="36.90625" customWidth="1"/>
-    <col min="3" max="3" width="36.7265625" customWidth="1"/>
-    <col min="4" max="4" width="39.6328125" customWidth="1"/>
-    <col min="5" max="5" width="26.7265625" customWidth="1"/>
-    <col min="6" max="6" width="24.36328125" customWidth="1"/>
-    <col min="7" max="7" width="22.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" customWidth="1"/>
+    <col min="4" max="4" width="17.08984375" customWidth="1"/>
+    <col min="5" max="5" width="15.08984375" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" customWidth="1"/>
     <col min="8" max="8" width="20.7265625" customWidth="1"/>
     <col min="9" max="9" width="16.08984375" customWidth="1"/>
   </cols>
@@ -1370,7 +1370,9 @@
       <c r="H1" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="I1" s="2"/>
+      <c r="I1" s="2" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
@@ -1391,10 +1393,10 @@
       <c r="F2" s="3">
         <v>12.6</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="8">
         <v>2.6</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="7">
         <v>2.8</v>
       </c>
     </row>
@@ -1417,10 +1419,10 @@
       <c r="F3" s="3">
         <v>15.5</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="8">
         <v>3.3</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="7">
         <v>3.6</v>
       </c>
     </row>
@@ -1443,10 +1445,10 @@
       <c r="F4" s="3">
         <v>15.5</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>5</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="7">
         <v>5.2</v>
       </c>
     </row>
@@ -1469,11 +1471,11 @@
       <c r="F5" s="3">
         <v>26.3</v>
       </c>
-      <c r="G5" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>121</v>
+      <c r="G5" s="8">
+        <v>23.8</v>
+      </c>
+      <c r="H5" s="8">
+        <v>24.5</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1495,11 +1497,11 @@
       <c r="F6" s="3">
         <v>30</v>
       </c>
-      <c r="G6" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>121</v>
+      <c r="G6" s="8">
+        <v>24.18</v>
+      </c>
+      <c r="H6" s="8">
+        <v>25.6</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1521,11 +1523,11 @@
       <c r="F7" s="3">
         <v>33.9</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>121</v>
+      <c r="G7" s="8">
+        <v>23.4</v>
+      </c>
+      <c r="H7" s="8">
+        <v>25.3</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1547,11 +1549,11 @@
       <c r="F8" s="3">
         <v>28.6</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>121</v>
+      <c r="G8" s="8">
+        <v>32.24</v>
+      </c>
+      <c r="H8" s="8">
+        <v>33.700000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1573,11 +1575,11 @@
       <c r="F9" s="3">
         <v>37.6</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>121</v>
+      <c r="G9" s="8">
+        <v>23.76</v>
+      </c>
+      <c r="H9" s="8">
+        <v>26.4</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1599,10 +1601,10 @@
       <c r="F10" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="8" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1625,11 +1627,11 @@
       <c r="F11" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>121</v>
+      <c r="G11" s="8">
+        <v>37.619999999999997</v>
+      </c>
+      <c r="H11" s="8">
+        <v>22.3</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1651,11 +1653,11 @@
       <c r="F12" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>121</v>
+      <c r="G12" s="8">
+        <v>54.15</v>
+      </c>
+      <c r="H12" s="8">
+        <v>55.7</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1677,11 +1679,11 @@
       <c r="F13" s="3">
         <v>26</v>
       </c>
-      <c r="G13" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>121</v>
+      <c r="G13" s="8">
+        <v>50.43</v>
+      </c>
+      <c r="H13" s="8">
+        <v>52.1</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1703,11 +1705,11 @@
       <c r="F14" s="3">
         <v>28</v>
       </c>
-      <c r="G14" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>121</v>
+      <c r="G14" s="8">
+        <v>57.4</v>
+      </c>
+      <c r="H14" s="8">
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1729,10 +1731,10 @@
       <c r="F15" s="3">
         <v>50</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="8">
         <v>61</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="8">
         <v>62.2</v>
       </c>
     </row>
@@ -1755,11 +1757,11 @@
       <c r="F16" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G16" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>121</v>
+      <c r="G16" s="8">
+        <v>66</v>
+      </c>
+      <c r="H16" s="8">
+        <v>68.3</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1781,11 +1783,11 @@
       <c r="F17" s="3">
         <v>44</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>121</v>
+      <c r="G17" s="8">
+        <v>111.28</v>
+      </c>
+      <c r="H17" s="8">
+        <v>113.4</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1807,11 +1809,11 @@
       <c r="F18" s="3">
         <v>49</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>121</v>
+      <c r="G18" s="8">
+        <v>87</v>
+      </c>
+      <c r="H18" s="8">
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1833,11 +1835,11 @@
       <c r="F19" s="3">
         <v>75</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>121</v>
+      <c r="G19" s="8">
+        <v>78.650000000000006</v>
+      </c>
+      <c r="H19" s="8">
+        <v>80.599999999999994</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1859,11 +1861,11 @@
       <c r="F20" s="3">
         <v>94</v>
       </c>
-      <c r="G20" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>121</v>
+      <c r="G20" s="8">
+        <v>119.31</v>
+      </c>
+      <c r="H20" s="8">
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1885,11 +1887,11 @@
       <c r="F21" s="3">
         <v>132</v>
       </c>
-      <c r="G21" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>121</v>
+      <c r="G21" s="8">
+        <v>147.84</v>
+      </c>
+      <c r="H21" s="8">
+        <v>108.5</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1911,11 +1913,11 @@
       <c r="F22" s="3">
         <v>118</v>
       </c>
-      <c r="G22" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>121</v>
+      <c r="G22" s="8">
+        <v>146.78</v>
+      </c>
+      <c r="H22" s="8">
+        <v>148.6</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1937,11 +1939,11 @@
       <c r="F23" s="3">
         <v>70.599999999999994</v>
       </c>
-      <c r="G23" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>121</v>
+      <c r="G23" s="8">
+        <v>171.6</v>
+      </c>
+      <c r="H23" s="8">
+        <v>122.55</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1963,11 +1965,11 @@
       <c r="F24" s="3">
         <v>77</v>
       </c>
-      <c r="G24" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>121</v>
+      <c r="G24" s="8">
+        <v>169.05</v>
+      </c>
+      <c r="H24" s="8">
+        <v>172.3</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1989,11 +1991,11 @@
       <c r="F25" s="3">
         <v>93</v>
       </c>
-      <c r="G25" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>121</v>
+      <c r="G25" s="8">
+        <v>205.8</v>
+      </c>
+      <c r="H25" s="8">
+        <v>207.8</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2015,11 +2017,11 @@
       <c r="F26" s="3">
         <v>93</v>
       </c>
-      <c r="G26" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>121</v>
+      <c r="G26" s="8">
+        <v>205.8</v>
+      </c>
+      <c r="H26" s="8">
+        <v>207.8</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2041,11 +2043,11 @@
       <c r="F27" s="3">
         <v>99</v>
       </c>
-      <c r="G27" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>121</v>
+      <c r="G27" s="8">
+        <v>256.04000000000002</v>
+      </c>
+      <c r="H27" s="8">
+        <v>172</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2067,11 +2069,11 @@
       <c r="F28" s="3">
         <v>99</v>
       </c>
-      <c r="G28" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>121</v>
+      <c r="G28" s="8">
+        <v>256.04000000000002</v>
+      </c>
+      <c r="H28" s="8">
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2093,11 +2095,11 @@
       <c r="F29" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G29" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>121</v>
+      <c r="G29" s="8">
+        <v>197.64</v>
+      </c>
+      <c r="H29" s="8">
+        <v>200.1</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2119,11 +2121,11 @@
       <c r="F30" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G30" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>121</v>
+      <c r="G30" s="8">
+        <v>197.64</v>
+      </c>
+      <c r="H30" s="8">
+        <v>200.1</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2145,11 +2147,11 @@
       <c r="F31" s="3">
         <v>113</v>
       </c>
-      <c r="G31" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>121</v>
+      <c r="G31" s="8">
+        <v>375.55</v>
+      </c>
+      <c r="H31" s="8">
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2171,11 +2173,11 @@
       <c r="F32" s="3">
         <v>140</v>
       </c>
-      <c r="G32" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>121</v>
+      <c r="G32" s="8">
+        <v>375.55</v>
+      </c>
+      <c r="H32" s="8">
+        <v>290</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2197,11 +2199,11 @@
       <c r="F33" s="3">
         <v>140</v>
       </c>
-      <c r="G33" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>121</v>
+      <c r="G33" s="8">
+        <v>375.55</v>
+      </c>
+      <c r="H33" s="8">
+        <v>290</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2223,11 +2225,11 @@
       <c r="F34" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="G34" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>121</v>
+      <c r="G34" s="8">
+        <v>281.77999999999997</v>
+      </c>
+      <c r="H34" s="8">
+        <v>284.7</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2249,11 +2251,11 @@
       <c r="F35" s="3">
         <v>150</v>
       </c>
-      <c r="G35" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>121</v>
+      <c r="G35" s="8">
+        <v>537.24</v>
+      </c>
+      <c r="H35" s="8">
+        <v>435</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2275,11 +2277,11 @@
       <c r="F36" s="3">
         <v>150</v>
       </c>
-      <c r="G36" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>121</v>
+      <c r="G36" s="8">
+        <v>537.24</v>
+      </c>
+      <c r="H36" s="8">
+        <v>435</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2301,11 +2303,11 @@
       <c r="F37" s="3">
         <v>230.5</v>
       </c>
-      <c r="G37" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>121</v>
+      <c r="G37" s="8">
+        <v>569.4</v>
+      </c>
+      <c r="H37" s="8">
+        <v>456</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2324,14 +2326,14 @@
       <c r="E38" s="3">
         <v>102000</v>
       </c>
-      <c r="F38" s="9">
+      <c r="F38" s="8">
         <v>230.5</v>
       </c>
-      <c r="G38" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>121</v>
+      <c r="G38" s="8">
+        <v>569.4</v>
+      </c>
+      <c r="H38" s="8">
+        <v>456</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2350,14 +2352,14 @@
       <c r="E39" s="3">
         <v>71800</v>
       </c>
-      <c r="F39" s="9" t="s">
+      <c r="F39" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G39" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>121</v>
+      <c r="G39" s="8">
+        <v>1079.73</v>
+      </c>
+      <c r="H39" s="8">
+        <v>1083.4000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2376,14 +2378,14 @@
       <c r="E40" s="3">
         <v>71800</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F40" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G40" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>121</v>
+      <c r="G40" s="8">
+        <v>1079.73</v>
+      </c>
+      <c r="H40" s="8">
+        <v>1083.4000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2402,14 +2404,14 @@
       <c r="E41" s="3">
         <v>201390</v>
       </c>
-      <c r="F41" s="9">
+      <c r="F41" s="8">
         <v>342</v>
       </c>
-      <c r="G41" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>121</v>
+      <c r="G41" s="8">
+        <v>2138.7024999999999</v>
+      </c>
+      <c r="H41" s="8">
+        <v>1754</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2428,14 +2430,14 @@
       <c r="E42" s="3">
         <v>166</v>
       </c>
-      <c r="F42" s="9">
+      <c r="F42" s="8">
         <v>23.1</v>
       </c>
-      <c r="G42" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>121</v>
+      <c r="G42" s="8">
+        <v>11.63</v>
+      </c>
+      <c r="H42" s="8">
+        <v>12.6</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2454,14 +2456,14 @@
       <c r="E43" s="3">
         <v>510</v>
       </c>
-      <c r="F43" s="9">
+      <c r="F43" s="8">
         <v>35.9</v>
       </c>
-      <c r="G43" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H43" s="9" t="s">
-        <v>121</v>
+      <c r="G43" s="8">
+        <v>31.35</v>
+      </c>
+      <c r="H43" s="8">
+        <v>15.5</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2480,14 +2482,14 @@
       <c r="E44" s="3">
         <v>1460</v>
       </c>
-      <c r="F44" s="9">
+      <c r="F44" s="8">
         <v>49.2</v>
       </c>
-      <c r="G44" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H44" s="9" t="s">
-        <v>121</v>
+      <c r="G44" s="8">
+        <v>50.05</v>
+      </c>
+      <c r="H44" s="8">
+        <v>28.1</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2506,14 +2508,14 @@
       <c r="E45" s="3">
         <v>3310</v>
       </c>
-      <c r="F45" s="9">
+      <c r="F45" s="8">
         <v>42.3</v>
       </c>
-      <c r="G45" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H45" s="9" t="s">
-        <v>121</v>
+      <c r="G45" s="8">
+        <v>67.89</v>
+      </c>
+      <c r="H45" s="8">
+        <v>40.700000000000003</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2532,14 +2534,14 @@
       <c r="E46" s="3">
         <v>4690</v>
       </c>
-      <c r="F46" s="9">
+      <c r="F46" s="8">
         <v>37.299999999999997</v>
       </c>
-      <c r="G46" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H46" s="9" t="s">
-        <v>121</v>
+      <c r="G46" s="8">
+        <v>87.36</v>
+      </c>
+      <c r="H46" s="8">
+        <v>52.3</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2558,14 +2560,14 @@
       <c r="E47" s="3">
         <v>296</v>
       </c>
-      <c r="F47" s="9" t="s">
+      <c r="F47" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G47" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H47" s="9" t="s">
-        <v>121</v>
+      <c r="G47" s="8">
+        <v>16</v>
+      </c>
+      <c r="H47" s="8">
+        <v>17.5</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2584,14 +2586,14 @@
       <c r="E48" s="3">
         <v>955</v>
       </c>
-      <c r="F48" s="9" t="s">
+      <c r="F48" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G48" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H48" s="9" t="s">
-        <v>121</v>
+      <c r="G48" s="8">
+        <v>20</v>
+      </c>
+      <c r="H48" s="8">
+        <v>21.4</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2610,14 +2612,14 @@
       <c r="E49" s="3">
         <v>2540</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F49" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G49" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H49" s="9" t="s">
-        <v>121</v>
+      <c r="G49" s="8">
+        <v>37.76</v>
+      </c>
+      <c r="H49" s="8">
+        <v>38.4</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2636,14 +2638,14 @@
       <c r="E50" s="3">
         <v>5390</v>
       </c>
-      <c r="F50" s="9" t="s">
+      <c r="F50" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G50" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H50" s="9" t="s">
-        <v>121</v>
+      <c r="G50" s="8">
+        <v>60.96</v>
+      </c>
+      <c r="H50" s="8">
+        <v>62.3</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2662,14 +2664,14 @@
       <c r="E51" s="3">
         <v>10200</v>
       </c>
-      <c r="F51" s="9" t="s">
+      <c r="F51" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G51" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H51" s="9" t="s">
-        <v>121</v>
+      <c r="G51" s="8">
+        <v>103.24</v>
+      </c>
+      <c r="H51" s="8">
+        <v>106.3</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2688,14 +2690,14 @@
       <c r="E52" s="3">
         <v>13748</v>
       </c>
-      <c r="F52" s="9" t="s">
+      <c r="F52" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G52" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H52" s="9" t="s">
-        <v>121</v>
+      <c r="G52" s="8">
+        <v>147.41999999999999</v>
+      </c>
+      <c r="H52" s="8">
+        <v>149.19999999999999</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2714,14 +2716,14 @@
       <c r="E53" s="3">
         <v>25000</v>
       </c>
-      <c r="F53" s="9" t="s">
+      <c r="F53" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G53" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H53" s="9" t="s">
-        <v>121</v>
+      <c r="G53" s="8">
+        <v>279.5</v>
+      </c>
+      <c r="H53" s="8">
+        <v>284.10000000000002</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2740,14 +2742,14 @@
       <c r="E54" s="3">
         <v>41500</v>
       </c>
-      <c r="F54" s="9" t="s">
+      <c r="F54" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G54" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H54" s="9" t="s">
-        <v>121</v>
+      <c r="G54" s="8">
+        <v>221.34</v>
+      </c>
+      <c r="H54" s="8">
+        <v>224.5</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2766,14 +2768,14 @@
       <c r="E55" s="3">
         <v>79410</v>
       </c>
-      <c r="F55" s="9" t="s">
+      <c r="F55" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G55" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H55" s="9" t="s">
-        <v>121</v>
+      <c r="G55" s="8">
+        <v>957.6</v>
+      </c>
+      <c r="H55" s="8">
+        <v>960.2</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2792,13 +2794,13 @@
       <c r="E56" s="3">
         <v>120</v>
       </c>
-      <c r="F56" s="9">
+      <c r="F56" s="8">
         <v>18.399999999999999</v>
       </c>
-      <c r="G56" s="9">
+      <c r="G56" s="8">
         <v>47.5</v>
       </c>
-      <c r="H56" s="7">
+      <c r="H56" s="6">
         <v>3.23</v>
       </c>
     </row>
@@ -2818,13 +2820,13 @@
       <c r="E57" s="3">
         <v>174</v>
       </c>
-      <c r="F57" s="9">
+      <c r="F57" s="8">
         <v>21.6</v>
       </c>
-      <c r="G57" s="9">
+      <c r="G57" s="8">
         <v>55</v>
       </c>
-      <c r="H57" s="7">
+      <c r="H57" s="6">
         <v>3.3</v>
       </c>
     </row>
@@ -2844,13 +2846,13 @@
       <c r="E58" s="3">
         <v>334</v>
       </c>
-      <c r="F58" s="9">
+      <c r="F58" s="8">
         <v>86</v>
       </c>
-      <c r="G58" s="9">
+      <c r="G58" s="8">
         <v>87</v>
       </c>
-      <c r="H58" s="9"/>
+      <c r="H58" s="8"/>
     </row>
     <row r="59" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="3" t="s">
@@ -2868,13 +2870,13 @@
       <c r="E59" s="3">
         <v>667</v>
       </c>
-      <c r="F59" s="9">
+      <c r="F59" s="8">
         <v>196</v>
       </c>
-      <c r="G59" s="9">
+      <c r="G59" s="8">
         <v>54</v>
       </c>
-      <c r="H59" s="7">
+      <c r="H59" s="6">
         <v>56.7</v>
       </c>
     </row>
@@ -2894,13 +2896,13 @@
       <c r="E60" s="3">
         <v>1640</v>
       </c>
-      <c r="F60" s="9">
+      <c r="F60" s="8">
         <v>225</v>
       </c>
-      <c r="G60" s="9">
+      <c r="G60" s="8">
         <v>115</v>
       </c>
-      <c r="H60" s="7">
+      <c r="H60" s="6">
         <v>117.8</v>
       </c>
     </row>
@@ -2920,13 +2922,13 @@
       <c r="E61" s="3">
         <v>1650</v>
       </c>
-      <c r="F61" s="9">
+      <c r="F61" s="8">
         <v>225</v>
       </c>
-      <c r="G61" s="9">
+      <c r="G61" s="8">
         <v>46.6</v>
       </c>
-      <c r="H61" s="7">
+      <c r="H61" s="6">
         <v>47.8</v>
       </c>
     </row>
@@ -2946,13 +2948,13 @@
       <c r="E62" s="3">
         <v>2414</v>
       </c>
-      <c r="F62" s="9">
+      <c r="F62" s="8">
         <v>225</v>
       </c>
-      <c r="G62" s="9">
+      <c r="G62" s="8">
         <v>90</v>
       </c>
-      <c r="H62" s="7">
+      <c r="H62" s="6">
         <v>93.2</v>
       </c>
     </row>
@@ -2972,13 +2974,13 @@
       <c r="E63" s="3">
         <v>2414</v>
       </c>
-      <c r="F63" s="9">
+      <c r="F63" s="8">
         <v>225</v>
       </c>
-      <c r="G63" s="9">
+      <c r="G63" s="8">
         <v>75</v>
       </c>
-      <c r="H63" s="7">
+      <c r="H63" s="6">
         <v>76.7</v>
       </c>
     </row>
@@ -2998,13 +3000,13 @@
       <c r="E64" s="3">
         <v>6400</v>
       </c>
-      <c r="F64" s="9" t="s">
+      <c r="F64" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G64" s="9">
+      <c r="G64" s="8">
         <v>187.5</v>
       </c>
-      <c r="H64" s="7">
+      <c r="H64" s="6">
         <v>190</v>
       </c>
     </row>
@@ -3024,13 +3026,13 @@
       <c r="E65" s="3">
         <v>3847</v>
       </c>
-      <c r="F65" s="9" t="s">
+      <c r="F65" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G65" s="9">
+      <c r="G65" s="8">
         <v>168</v>
       </c>
-      <c r="H65" s="7">
+      <c r="H65" s="6">
         <v>170.2</v>
       </c>
     </row>
@@ -3050,13 +3052,13 @@
       <c r="E66" s="3">
         <v>9950</v>
       </c>
-      <c r="F66" s="9" t="s">
+      <c r="F66" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G66" s="9">
+      <c r="G66" s="8">
         <v>220</v>
       </c>
-      <c r="H66" s="7">
+      <c r="H66" s="6">
         <v>223.4</v>
       </c>
     </row>
@@ -3076,13 +3078,13 @@
       <c r="E67" s="3">
         <v>16800</v>
       </c>
-      <c r="F67" s="9" t="s">
+      <c r="F67" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G67" s="9">
+      <c r="G67" s="8">
         <v>462</v>
       </c>
-      <c r="H67" s="7">
+      <c r="H67" s="6">
         <v>463.2</v>
       </c>
     </row>
@@ -3102,13 +3104,13 @@
       <c r="E68" s="3">
         <v>18400</v>
       </c>
-      <c r="F68" s="9" t="s">
+      <c r="F68" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G68" s="9">
+      <c r="G68" s="8">
         <v>414</v>
       </c>
-      <c r="H68" s="7">
+      <c r="H68" s="6">
         <v>415.6</v>
       </c>
     </row>
@@ -3128,13 +3130,13 @@
       <c r="E69" s="3">
         <v>28700</v>
       </c>
-      <c r="F69" s="9" t="s">
+      <c r="F69" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G69" s="9">
+      <c r="G69" s="8">
         <v>567</v>
       </c>
-      <c r="H69" s="7">
+      <c r="H69" s="6">
         <v>567.9</v>
       </c>
     </row>
@@ -3154,13 +3156,13 @@
       <c r="E70" s="3">
         <v>23000</v>
       </c>
-      <c r="F70" s="9" t="s">
+      <c r="F70" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G70" s="9">
+      <c r="G70" s="8">
         <v>972</v>
       </c>
-      <c r="H70" s="7">
+      <c r="H70" s="6">
         <v>973</v>
       </c>
     </row>
@@ -3180,13 +3182,13 @@
       <c r="E71" s="3">
         <v>347</v>
       </c>
-      <c r="F71" s="9" t="s">
+      <c r="F71" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G71" s="9">
+      <c r="G71" s="8">
         <v>36.6</v>
       </c>
-      <c r="H71" s="7">
+      <c r="H71" s="6">
         <v>38.4</v>
       </c>
     </row>
@@ -3206,13 +3208,13 @@
       <c r="E72" s="3">
         <v>347</v>
       </c>
-      <c r="F72" s="9" t="s">
+      <c r="F72" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G72" s="9">
+      <c r="G72" s="8">
         <v>12.8</v>
       </c>
-      <c r="H72" s="7">
+      <c r="H72" s="6">
         <v>13.1</v>
       </c>
     </row>
@@ -3232,13 +3234,13 @@
       <c r="E73" s="3">
         <v>1960</v>
       </c>
-      <c r="F73" s="9" t="s">
+      <c r="F73" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G73" s="9">
+      <c r="G73" s="8">
         <v>125.4</v>
       </c>
-      <c r="H73" s="7">
+      <c r="H73" s="6">
         <v>126.8</v>
       </c>
     </row>
@@ -3258,13 +3260,13 @@
       <c r="E74" s="3">
         <v>1960</v>
       </c>
-      <c r="F74" s="9" t="s">
+      <c r="F74" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G74" s="9">
+      <c r="G74" s="8">
         <v>46.6</v>
       </c>
-      <c r="H74" s="7">
+      <c r="H74" s="6">
         <v>48</v>
       </c>
     </row>
@@ -3284,13 +3286,13 @@
       <c r="E75" s="3">
         <v>3082</v>
       </c>
-      <c r="F75" s="9" t="s">
+      <c r="F75" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G75" s="9">
+      <c r="G75" s="8">
         <v>140.80000000000001</v>
       </c>
-      <c r="H75" s="7">
+      <c r="H75" s="6">
         <v>142.1</v>
       </c>
     </row>
@@ -3310,13 +3312,13 @@
       <c r="E76" s="3">
         <v>3082</v>
       </c>
-      <c r="F76" s="9" t="s">
+      <c r="F76" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G76" s="9">
+      <c r="G76" s="8">
         <v>57.8</v>
       </c>
-      <c r="H76" s="7">
+      <c r="H76" s="6">
         <v>59.3</v>
       </c>
     </row>
@@ -3336,13 +3338,13 @@
       <c r="E77" s="3">
         <v>4970</v>
       </c>
-      <c r="F77" s="9" t="s">
+      <c r="F77" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G77" s="9">
+      <c r="G77" s="8">
         <v>240</v>
       </c>
-      <c r="H77" s="7">
+      <c r="H77" s="6">
         <v>243</v>
       </c>
     </row>
@@ -3362,13 +3364,13 @@
       <c r="E78" s="3">
         <v>3400</v>
       </c>
-      <c r="F78" s="9" t="s">
+      <c r="F78" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="G78" s="9">
+      <c r="G78" s="8">
         <v>81</v>
       </c>
-      <c r="H78" s="7">
+      <c r="H78" s="6">
         <v>83</v>
       </c>
     </row>
@@ -3388,14 +3390,14 @@
       <c r="E79" s="3">
         <v>251</v>
       </c>
-      <c r="F79" s="9">
+      <c r="F79" s="8">
         <v>20.100000000000001</v>
       </c>
-      <c r="G79" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="H79" s="9" t="s">
-        <v>121</v>
+      <c r="G79" s="8">
+        <v>14</v>
+      </c>
+      <c r="H79" s="8">
+        <v>4.7</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3414,13 +3416,13 @@
       <c r="E80" s="3">
         <v>430</v>
       </c>
-      <c r="F80" s="9">
+      <c r="F80" s="8">
         <v>25</v>
       </c>
       <c r="G80" s="3">
         <v>12.6</v>
       </c>
-      <c r="H80" s="6">
+      <c r="H80" s="5">
         <v>9.5</v>
       </c>
     </row>
@@ -3440,13 +3442,13 @@
       <c r="E81" s="3">
         <v>820</v>
       </c>
-      <c r="F81" s="9">
+      <c r="F81" s="8">
         <v>30</v>
       </c>
       <c r="G81" s="3">
         <v>24</v>
       </c>
-      <c r="H81" s="6">
+      <c r="H81" s="5">
         <v>15</v>
       </c>
     </row>
@@ -3466,13 +3468,13 @@
       <c r="E82" s="3">
         <v>1060</v>
       </c>
-      <c r="F82" s="9">
+      <c r="F82" s="8">
         <v>35</v>
       </c>
       <c r="G82" s="3">
         <v>25.2</v>
       </c>
-      <c r="H82" s="7">
+      <c r="H82" s="6">
         <v>22.4</v>
       </c>
     </row>
@@ -3492,13 +3494,13 @@
       <c r="E83" s="3">
         <v>1860</v>
       </c>
-      <c r="F83" s="9">
+      <c r="F83" s="8">
         <v>42</v>
       </c>
       <c r="G83" s="3">
         <v>47.5</v>
       </c>
-      <c r="H83" s="6">
+      <c r="H83" s="5">
         <v>30</v>
       </c>
     </row>
@@ -3518,13 +3520,13 @@
       <c r="E84" s="3">
         <v>3360</v>
       </c>
-      <c r="F84" s="9">
+      <c r="F84" s="8">
         <v>47</v>
       </c>
       <c r="G84" s="3">
         <v>66.900000000000006</v>
       </c>
-      <c r="H84" s="8">
+      <c r="H84" s="7">
         <v>41.5</v>
       </c>
     </row>
@@ -3544,13 +3546,13 @@
       <c r="E85" s="3">
         <v>6195</v>
       </c>
-      <c r="F85" s="9">
+      <c r="F85" s="8">
         <v>50</v>
       </c>
       <c r="G85" s="3">
         <v>102.5</v>
       </c>
-      <c r="H85" s="8">
+      <c r="H85" s="7">
         <v>73</v>
       </c>
     </row>
@@ -3570,13 +3572,13 @@
       <c r="E86" s="3">
         <v>10230</v>
       </c>
-      <c r="F86" s="9">
+      <c r="F86" s="8">
         <v>50</v>
       </c>
       <c r="G86" s="3">
         <v>145.6</v>
       </c>
-      <c r="H86" s="8">
+      <c r="H86" s="7">
         <v>107</v>
       </c>
     </row>
@@ -3596,13 +3598,13 @@
       <c r="E87" s="3">
         <v>31000</v>
       </c>
-      <c r="F87" s="9">
+      <c r="F87" s="8">
         <v>96.8</v>
       </c>
       <c r="G87" s="3">
         <v>189.8</v>
       </c>
-      <c r="H87" s="8">
+      <c r="H87" s="7">
         <v>154</v>
       </c>
     </row>
@@ -3622,13 +3624,13 @@
       <c r="E88" s="3">
         <v>62000</v>
       </c>
-      <c r="F88" s="9">
+      <c r="F88" s="8">
         <v>120</v>
       </c>
       <c r="G88" s="3">
         <v>335.7</v>
       </c>
-      <c r="H88" s="8">
+      <c r="H88" s="7">
         <v>270</v>
       </c>
     </row>
@@ -3648,13 +3650,13 @@
       <c r="E89" s="3">
         <v>101000</v>
       </c>
-      <c r="F89" s="9">
+      <c r="F89" s="8">
         <v>140</v>
       </c>
       <c r="G89" s="3">
         <v>490.4</v>
       </c>
-      <c r="H89" s="8">
+      <c r="H89" s="7">
         <v>442</v>
       </c>
     </row>
@@ -3674,13 +3676,13 @@
       <c r="E90" s="3">
         <v>133000</v>
       </c>
-      <c r="F90" s="9">
+      <c r="F90" s="8">
         <v>158</v>
       </c>
       <c r="G90" s="3">
         <v>556.79999999999995</v>
       </c>
-      <c r="H90" s="8">
+      <c r="H90" s="7">
         <v>657</v>
       </c>
     </row>
@@ -3700,13 +3702,13 @@
       <c r="E91" s="3">
         <v>344000</v>
       </c>
-      <c r="F91" s="9">
+      <c r="F91" s="8">
         <v>210</v>
       </c>
       <c r="G91" s="3">
         <v>1184.4000000000001</v>
       </c>
-      <c r="H91" s="8">
+      <c r="H91" s="7">
         <v>1070</v>
       </c>
     </row>
@@ -3726,13 +3728,13 @@
       <c r="E92" s="3">
         <v>7</v>
       </c>
-      <c r="F92" s="9">
+      <c r="F92" s="8">
         <v>5.8</v>
       </c>
       <c r="G92" s="3">
         <v>1.02</v>
       </c>
-      <c r="H92" s="8">
+      <c r="H92" s="7">
         <v>0.65</v>
       </c>
     </row>
@@ -3752,13 +3754,13 @@
       <c r="E93" s="3">
         <v>21.3</v>
       </c>
-      <c r="F93" s="9" t="s">
+      <c r="F93" s="8" t="s">
         <v>121</v>
       </c>
       <c r="G93" s="3">
         <v>3.7</v>
       </c>
-      <c r="H93" s="8">
+      <c r="H93" s="7">
         <v>3.94</v>
       </c>
     </row>
@@ -3778,13 +3780,13 @@
       <c r="E94" s="3">
         <v>37</v>
       </c>
-      <c r="F94" s="9" t="s">
+      <c r="F94" s="8" t="s">
         <v>121</v>
       </c>
       <c r="G94" s="3">
         <v>1.7</v>
       </c>
-      <c r="H94" s="8">
+      <c r="H94" s="7">
         <v>1.9</v>
       </c>
     </row>
@@ -3804,13 +3806,13 @@
       <c r="E95" s="3">
         <v>70</v>
       </c>
-      <c r="F95" s="9">
+      <c r="F95" s="8">
         <v>14.6</v>
       </c>
       <c r="G95" s="3">
         <v>2.2400000000000002</v>
       </c>
-      <c r="H95" s="8">
+      <c r="H95" s="7">
         <v>2.2000000000000002</v>
       </c>
     </row>
@@ -3830,13 +3832,13 @@
       <c r="E96" s="3">
         <v>125</v>
       </c>
-      <c r="F96" s="9">
+      <c r="F96" s="8">
         <v>19.2</v>
       </c>
       <c r="G96" s="3">
         <v>5.04</v>
       </c>
-      <c r="H96" s="8">
+      <c r="H96" s="7">
         <v>3.6</v>
       </c>
     </row>
@@ -3856,13 +3858,13 @@
       <c r="E97" s="3">
         <v>253</v>
       </c>
-      <c r="F97" s="9">
+      <c r="F97" s="8">
         <v>22</v>
       </c>
       <c r="G97" s="3">
         <v>8.8000000000000007</v>
       </c>
-      <c r="H97" s="8">
+      <c r="H97" s="7">
         <v>4.2</v>
       </c>
     </row>
@@ -3888,7 +3890,7 @@
       <c r="G98" s="3">
         <v>16.8</v>
       </c>
-      <c r="H98" s="8">
+      <c r="H98" s="7">
         <v>8.4</v>
       </c>
     </row>
@@ -3914,7 +3916,7 @@
       <c r="G99" s="3">
         <v>16.600000000000001</v>
       </c>
-      <c r="H99" s="8">
+      <c r="H99" s="7">
         <v>16</v>
       </c>
     </row>
@@ -3940,7 +3942,7 @@
       <c r="G100" s="3">
         <v>23</v>
       </c>
-      <c r="H100" s="8">
+      <c r="H100" s="7">
         <v>23.4</v>
       </c>
     </row>
@@ -3966,7 +3968,7 @@
       <c r="G101" s="3">
         <v>33.6</v>
       </c>
-      <c r="H101" s="8">
+      <c r="H101" s="7">
         <v>32</v>
       </c>
     </row>
@@ -3992,7 +3994,7 @@
       <c r="G102" s="3">
         <v>52.6</v>
       </c>
-      <c r="H102" s="8">
+      <c r="H102" s="7">
         <v>48</v>
       </c>
     </row>
@@ -4018,7 +4020,7 @@
       <c r="G103" s="3">
         <v>78.84</v>
       </c>
-      <c r="H103" s="8">
+      <c r="H103" s="7">
         <v>63</v>
       </c>
     </row>
@@ -4044,7 +4046,7 @@
       <c r="G104" s="3">
         <v>102</v>
       </c>
-      <c r="H104" s="8">
+      <c r="H104" s="7">
         <v>104.2</v>
       </c>
     </row>
@@ -4070,7 +4072,7 @@
       <c r="G105" s="3">
         <v>137.75</v>
       </c>
-      <c r="H105" s="8">
+      <c r="H105" s="7">
         <v>139.6</v>
       </c>
     </row>
@@ -4096,7 +4098,7 @@
       <c r="G106" s="3">
         <v>31.49</v>
       </c>
-      <c r="H106" s="8">
+      <c r="H106" s="7">
         <v>33.6</v>
       </c>
     </row>
@@ -4122,7 +4124,7 @@
       <c r="G107" s="3">
         <v>45.32</v>
       </c>
-      <c r="H107" s="8">
+      <c r="H107" s="7">
         <v>47.2</v>
       </c>
     </row>
@@ -4148,7 +4150,7 @@
       <c r="G108" s="3">
         <v>83.6</v>
       </c>
-      <c r="H108" s="8">
+      <c r="H108" s="7">
         <v>84.5</v>
       </c>
     </row>
@@ -4174,7 +4176,7 @@
       <c r="G109" s="3">
         <v>83.4</v>
       </c>
-      <c r="H109" s="8">
+      <c r="H109" s="7">
         <v>33</v>
       </c>
     </row>
@@ -4200,7 +4202,7 @@
       <c r="G110" s="3">
         <v>96.6</v>
       </c>
-      <c r="H110" s="8">
+      <c r="H110" s="7">
         <v>47</v>
       </c>
     </row>
@@ -4226,7 +4228,7 @@
       <c r="G111" s="3">
         <v>106.7</v>
       </c>
-      <c r="H111" s="8">
+      <c r="H111" s="7">
         <v>47</v>
       </c>
     </row>
@@ -4252,7 +4254,7 @@
       <c r="G112" s="3">
         <v>143.19999999999999</v>
       </c>
-      <c r="H112" s="8">
+      <c r="H112" s="7">
         <v>104</v>
       </c>
     </row>
@@ -4278,7 +4280,7 @@
       <c r="G113" s="3">
         <v>197.03</v>
       </c>
-      <c r="H113" s="8">
+      <c r="H113" s="7">
         <v>158</v>
       </c>
     </row>
@@ -4304,7 +4306,7 @@
       <c r="G114" s="3">
         <v>377.6</v>
       </c>
-      <c r="H114" s="8">
+      <c r="H114" s="7">
         <v>309</v>
       </c>
     </row>
@@ -4330,7 +4332,7 @@
       <c r="G115" s="3">
         <v>540</v>
       </c>
-      <c r="H115" s="8">
+      <c r="H115" s="7">
         <v>340</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added values to the mean length of turn column
</commit_message>
<xml_diff>
--- a/Cores-Info-Database.xlsx
+++ b/Cores-Info-Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19725\Desktop\education\college\extracurriculars\pemg research\PEMG_Design_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E17DD71-7354-467E-AD78-6B7758038915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A399FC-D2E3-4BE6-89A8-2AE1DE7954D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{FD5E7F2C-425F-4B8A-9B1F-7669120DD1D5}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="126">
   <si>
     <t>E 5</t>
   </si>
@@ -395,6 +395,9 @@
   </si>
   <si>
     <t>l_N</t>
+  </si>
+  <si>
+    <t>Not Available</t>
   </si>
 </sst>
 </file>
@@ -925,7 +928,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -949,6 +952,15 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1328,8 +1340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50AB67D-9472-4E0F-AB22-86EA84CCBB8E}">
   <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1399,6 +1411,9 @@
       <c r="H2" s="7">
         <v>2.8</v>
       </c>
+      <c r="I2" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
@@ -1425,6 +1440,9 @@
       <c r="H3" s="7">
         <v>3.6</v>
       </c>
+      <c r="I3" s="9">
+        <v>12.8</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
@@ -1451,6 +1469,9 @@
       <c r="H4" s="7">
         <v>5.2</v>
       </c>
+      <c r="I4" s="9">
+        <v>14.9</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
@@ -1477,6 +1498,9 @@
       <c r="H5" s="8">
         <v>24.5</v>
       </c>
+      <c r="I5" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
@@ -1503,6 +1527,9 @@
       <c r="H6" s="8">
         <v>25.6</v>
       </c>
+      <c r="I6" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
@@ -1529,6 +1556,9 @@
       <c r="H7" s="8">
         <v>25.3</v>
       </c>
+      <c r="I7" s="10">
+        <v>11.6</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
@@ -1555,6 +1585,9 @@
       <c r="H8" s="8">
         <v>33.700000000000003</v>
       </c>
+      <c r="I8" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
@@ -1581,6 +1614,9 @@
       <c r="H9" s="8">
         <v>26.4</v>
       </c>
+      <c r="I9" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
@@ -1607,6 +1643,9 @@
       <c r="H10" s="8" t="s">
         <v>121</v>
       </c>
+      <c r="I10" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
@@ -1633,6 +1672,9 @@
       <c r="H11" s="8">
         <v>22.3</v>
       </c>
+      <c r="I11" s="10">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
@@ -1659,6 +1701,9 @@
       <c r="H12" s="8">
         <v>55.7</v>
       </c>
+      <c r="I12" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
@@ -1685,6 +1730,9 @@
       <c r="H13" s="8">
         <v>52.1</v>
       </c>
+      <c r="I13" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
@@ -1711,6 +1759,9 @@
       <c r="H14" s="8">
         <v>34</v>
       </c>
+      <c r="I14" s="10">
+        <v>41.2</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
@@ -1737,6 +1788,9 @@
       <c r="H15" s="8">
         <v>62.2</v>
       </c>
+      <c r="I15" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
@@ -1763,8 +1817,11 @@
       <c r="H16" s="8">
         <v>68.3</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1789,8 +1846,11 @@
       <c r="H17" s="8">
         <v>113.4</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -1815,8 +1875,11 @@
       <c r="H18" s="8">
         <v>61</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I18" s="10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -1841,8 +1904,11 @@
       <c r="H19" s="8">
         <v>80.599999999999994</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
@@ -1867,8 +1933,11 @@
       <c r="H20" s="8">
         <v>90</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I20" s="10">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -1893,8 +1962,11 @@
       <c r="H21" s="8">
         <v>108.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I21" s="10">
+        <v>92.6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -1919,8 +1991,11 @@
       <c r="H22" s="8">
         <v>148.6</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
@@ -1945,8 +2020,11 @@
       <c r="H23" s="8">
         <v>122.55</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I23" s="10">
+        <v>76.400000000000006</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
@@ -1971,8 +2049,11 @@
       <c r="H24" s="8">
         <v>172.3</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -1997,8 +2078,11 @@
       <c r="H25" s="8">
         <v>207.8</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I25" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
@@ -2023,8 +2107,11 @@
       <c r="H26" s="8">
         <v>207.8</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
@@ -2049,8 +2136,11 @@
       <c r="H27" s="8">
         <v>172</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I27" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
@@ -2075,8 +2165,11 @@
       <c r="H28" s="8">
         <v>172</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I28" s="10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
@@ -2101,8 +2194,11 @@
       <c r="H29" s="8">
         <v>200.1</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
@@ -2127,8 +2223,11 @@
       <c r="H30" s="8">
         <v>200.1</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
@@ -2153,8 +2252,11 @@
       <c r="H31" s="8">
         <v>280</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I31" s="10">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>30</v>
       </c>
@@ -2179,8 +2281,11 @@
       <c r="H32" s="8">
         <v>290</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I32" s="10">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
@@ -2205,8 +2310,11 @@
       <c r="H33" s="8">
         <v>290</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I33" s="10">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="3" t="s">
         <v>32</v>
       </c>
@@ -2231,8 +2339,11 @@
       <c r="H34" s="8">
         <v>284.7</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
         <v>33</v>
       </c>
@@ -2257,8 +2368,11 @@
       <c r="H35" s="8">
         <v>435</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I35" s="10">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="3" t="s">
         <v>34</v>
       </c>
@@ -2283,8 +2397,11 @@
       <c r="H36" s="8">
         <v>435</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I36" s="10">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
         <v>35</v>
       </c>
@@ -2309,8 +2426,11 @@
       <c r="H37" s="8">
         <v>456</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I37" s="10">
+        <v>230.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
@@ -2335,8 +2455,11 @@
       <c r="H38" s="8">
         <v>456</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I38" s="10">
+        <v>230.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="3" t="s">
         <v>37</v>
       </c>
@@ -2361,8 +2484,11 @@
       <c r="H39" s="8">
         <v>1083.4000000000001</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I39" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="3" t="s">
         <v>38</v>
       </c>
@@ -2387,8 +2513,11 @@
       <c r="H40" s="8">
         <v>1083.4000000000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I40" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="3" t="s">
         <v>39</v>
       </c>
@@ -2413,8 +2542,11 @@
       <c r="H41" s="8">
         <v>1754</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I41" s="10">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="3" t="s">
         <v>40</v>
       </c>
@@ -2439,8 +2571,11 @@
       <c r="H42" s="8">
         <v>12.6</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="3" t="s">
         <v>41</v>
       </c>
@@ -2465,8 +2600,11 @@
       <c r="H43" s="8">
         <v>15.5</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I43" s="11">
+        <v>35.9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="3" t="s">
         <v>42</v>
       </c>
@@ -2491,8 +2629,11 @@
       <c r="H44" s="8">
         <v>28.1</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I44" s="11">
+        <v>40.200000000000003</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="3" t="s">
         <v>43</v>
       </c>
@@ -2517,8 +2658,11 @@
       <c r="H45" s="8">
         <v>40.700000000000003</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I45" s="11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="3" t="s">
         <v>44</v>
       </c>
@@ -2543,8 +2687,11 @@
       <c r="H46" s="8">
         <v>52.3</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I46" s="11">
+        <v>56.7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="3" t="s">
         <v>45</v>
       </c>
@@ -2569,8 +2716,11 @@
       <c r="H47" s="8">
         <v>17.5</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I47" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="3" t="s">
         <v>46</v>
       </c>
@@ -2595,8 +2745,11 @@
       <c r="H48" s="8">
         <v>21.4</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I48" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="3" t="s">
         <v>47</v>
       </c>
@@ -2621,8 +2774,11 @@
       <c r="H49" s="8">
         <v>38.4</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I49" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="3" t="s">
         <v>48</v>
       </c>
@@ -2647,8 +2803,11 @@
       <c r="H50" s="8">
         <v>62.3</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I50" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="3" t="s">
         <v>49</v>
       </c>
@@ -2673,8 +2832,11 @@
       <c r="H51" s="8">
         <v>106.3</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I51" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="3" t="s">
         <v>50</v>
       </c>
@@ -2699,8 +2861,11 @@
       <c r="H52" s="8">
         <v>149.19999999999999</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I52" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="3" t="s">
         <v>51</v>
       </c>
@@ -2725,8 +2890,11 @@
       <c r="H53" s="8">
         <v>284.10000000000002</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I53" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="3" t="s">
         <v>52</v>
       </c>
@@ -2751,8 +2919,11 @@
       <c r="H54" s="8">
         <v>224.5</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I54" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="3" t="s">
         <v>53</v>
       </c>
@@ -2777,8 +2948,11 @@
       <c r="H55" s="8">
         <v>960.2</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I55" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="3" t="s">
         <v>54</v>
       </c>
@@ -2803,8 +2977,11 @@
       <c r="H56" s="6">
         <v>3.23</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I56" s="10">
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="3" t="s">
         <v>55</v>
       </c>
@@ -2829,8 +3006,11 @@
       <c r="H57" s="6">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I57" s="10">
+        <v>21.6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="3" t="s">
         <v>56</v>
       </c>
@@ -2852,9 +3032,14 @@
       <c r="G58" s="8">
         <v>87</v>
       </c>
-      <c r="H58" s="8"/>
-    </row>
-    <row r="59" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="H58" s="8">
+        <v>88.9</v>
+      </c>
+      <c r="I58" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="3" t="s">
         <v>57</v>
       </c>
@@ -2879,8 +3064,11 @@
       <c r="H59" s="6">
         <v>56.7</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I59" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="3" t="s">
         <v>58</v>
       </c>
@@ -2905,8 +3093,11 @@
       <c r="H60" s="6">
         <v>117.8</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I60" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="3" t="s">
         <v>59</v>
       </c>
@@ -2931,8 +3122,11 @@
       <c r="H61" s="6">
         <v>47.8</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I61" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="3" t="s">
         <v>60</v>
       </c>
@@ -2957,8 +3151,11 @@
       <c r="H62" s="6">
         <v>93.2</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I62" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="3" t="s">
         <v>61</v>
       </c>
@@ -2983,8 +3180,11 @@
       <c r="H63" s="6">
         <v>76.7</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I63" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="3" t="s">
         <v>62</v>
       </c>
@@ -3009,8 +3209,11 @@
       <c r="H64" s="6">
         <v>190</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I64" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="3" t="s">
         <v>63</v>
       </c>
@@ -3035,8 +3238,11 @@
       <c r="H65" s="6">
         <v>170.2</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I65" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="3" t="s">
         <v>64</v>
       </c>
@@ -3061,8 +3267,11 @@
       <c r="H66" s="6">
         <v>223.4</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I66" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" s="3" t="s">
         <v>65</v>
       </c>
@@ -3087,8 +3296,11 @@
       <c r="H67" s="6">
         <v>463.2</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I67" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="3" t="s">
         <v>66</v>
       </c>
@@ -3113,8 +3325,11 @@
       <c r="H68" s="6">
         <v>415.6</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I68" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="3" t="s">
         <v>67</v>
       </c>
@@ -3139,8 +3354,11 @@
       <c r="H69" s="6">
         <v>567.9</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I69" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="3" t="s">
         <v>68</v>
       </c>
@@ -3165,8 +3383,11 @@
       <c r="H70" s="6">
         <v>973</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I70" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="3" t="s">
         <v>69</v>
       </c>
@@ -3192,7 +3413,7 @@
         <v>38.4</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A72" s="3" t="s">
         <v>70</v>
       </c>
@@ -3218,7 +3439,7 @@
         <v>13.1</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="3" t="s">
         <v>71</v>
       </c>
@@ -3244,7 +3465,7 @@
         <v>126.8</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="3" t="s">
         <v>72</v>
       </c>
@@ -3270,7 +3491,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="3" t="s">
         <v>73</v>
       </c>
@@ -3296,7 +3517,7 @@
         <v>142.1</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="3" t="s">
         <v>74</v>
       </c>
@@ -3322,7 +3543,7 @@
         <v>59.3</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="3" t="s">
         <v>75</v>
       </c>
@@ -3348,7 +3569,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="3" t="s">
         <v>76</v>
       </c>
@@ -3374,7 +3595,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="3" t="s">
         <v>77</v>
       </c>
@@ -3400,7 +3621,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="3" t="s">
         <v>106</v>
       </c>

</xml_diff>

<commit_message>
Added the mean length of turn
</commit_message>
<xml_diff>
--- a/Cores-Info-Database.xlsx
+++ b/Cores-Info-Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19725\Desktop\education\college\extracurriculars\pemg research\PEMG_Design_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A399FC-D2E3-4BE6-89A8-2AE1DE7954D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AC8855-9782-4822-9E55-ADC660530542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{FD5E7F2C-425F-4B8A-9B1F-7669120DD1D5}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="126">
   <si>
     <t>E 5</t>
   </si>
@@ -928,7 +928,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -954,14 +954,17 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1340,8 +1343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50AB67D-9472-4E0F-AB22-86EA84CCBB8E}">
   <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="I71" sqref="I71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I116" sqref="I116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1440,7 +1443,7 @@
       <c r="H3" s="7">
         <v>3.6</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="7">
         <v>12.8</v>
       </c>
     </row>
@@ -1469,7 +1472,7 @@
       <c r="H4" s="7">
         <v>5.2</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="7">
         <v>14.9</v>
       </c>
     </row>
@@ -1556,7 +1559,7 @@
       <c r="H7" s="8">
         <v>25.3</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="6">
         <v>11.6</v>
       </c>
     </row>
@@ -1672,7 +1675,7 @@
       <c r="H11" s="8">
         <v>22.3</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="6">
         <v>34</v>
       </c>
     </row>
@@ -1759,7 +1762,7 @@
       <c r="H14" s="8">
         <v>34</v>
       </c>
-      <c r="I14" s="10">
+      <c r="I14" s="6">
         <v>41.2</v>
       </c>
     </row>
@@ -1875,7 +1878,7 @@
       <c r="H18" s="8">
         <v>61</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="6">
         <v>50</v>
       </c>
     </row>
@@ -1933,7 +1936,7 @@
       <c r="H20" s="8">
         <v>90</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="6">
         <v>56</v>
       </c>
     </row>
@@ -1962,7 +1965,7 @@
       <c r="H21" s="8">
         <v>108.5</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="6">
         <v>92.6</v>
       </c>
     </row>
@@ -2020,7 +2023,7 @@
       <c r="H23" s="8">
         <v>122.55</v>
       </c>
-      <c r="I23" s="10">
+      <c r="I23" s="6">
         <v>76.400000000000006</v>
       </c>
     </row>
@@ -2136,7 +2139,7 @@
       <c r="H27" s="8">
         <v>172</v>
       </c>
-      <c r="I27" s="10">
+      <c r="I27" s="6">
         <v>100</v>
       </c>
     </row>
@@ -2165,7 +2168,7 @@
       <c r="H28" s="8">
         <v>172</v>
       </c>
-      <c r="I28" s="10">
+      <c r="I28" s="6">
         <v>100</v>
       </c>
     </row>
@@ -2252,7 +2255,7 @@
       <c r="H31" s="8">
         <v>280</v>
       </c>
-      <c r="I31" s="10">
+      <c r="I31" s="6">
         <v>113</v>
       </c>
     </row>
@@ -2281,7 +2284,7 @@
       <c r="H32" s="8">
         <v>290</v>
       </c>
-      <c r="I32" s="10">
+      <c r="I32" s="6">
         <v>140</v>
       </c>
     </row>
@@ -2310,7 +2313,7 @@
       <c r="H33" s="8">
         <v>290</v>
       </c>
-      <c r="I33" s="10">
+      <c r="I33" s="6">
         <v>140</v>
       </c>
     </row>
@@ -2368,7 +2371,7 @@
       <c r="H35" s="8">
         <v>435</v>
       </c>
-      <c r="I35" s="10">
+      <c r="I35" s="6">
         <v>246</v>
       </c>
     </row>
@@ -2397,7 +2400,7 @@
       <c r="H36" s="8">
         <v>435</v>
       </c>
-      <c r="I36" s="10">
+      <c r="I36" s="6">
         <v>246</v>
       </c>
     </row>
@@ -2426,7 +2429,7 @@
       <c r="H37" s="8">
         <v>456</v>
       </c>
-      <c r="I37" s="10">
+      <c r="I37" s="6">
         <v>230.5</v>
       </c>
     </row>
@@ -2455,7 +2458,7 @@
       <c r="H38" s="8">
         <v>456</v>
       </c>
-      <c r="I38" s="10">
+      <c r="I38" s="6">
         <v>230.5</v>
       </c>
     </row>
@@ -2542,7 +2545,7 @@
       <c r="H41" s="8">
         <v>1754</v>
       </c>
-      <c r="I41" s="10">
+      <c r="I41" s="6">
         <v>342</v>
       </c>
     </row>
@@ -2600,7 +2603,7 @@
       <c r="H43" s="8">
         <v>15.5</v>
       </c>
-      <c r="I43" s="11">
+      <c r="I43" s="8">
         <v>35.9</v>
       </c>
     </row>
@@ -2629,7 +2632,7 @@
       <c r="H44" s="8">
         <v>28.1</v>
       </c>
-      <c r="I44" s="11">
+      <c r="I44" s="8">
         <v>40.200000000000003</v>
       </c>
     </row>
@@ -2658,7 +2661,7 @@
       <c r="H45" s="8">
         <v>40.700000000000003</v>
       </c>
-      <c r="I45" s="11">
+      <c r="I45" s="8">
         <v>50</v>
       </c>
     </row>
@@ -2687,7 +2690,7 @@
       <c r="H46" s="8">
         <v>52.3</v>
       </c>
-      <c r="I46" s="11">
+      <c r="I46" s="8">
         <v>56.7</v>
       </c>
     </row>
@@ -2977,7 +2980,7 @@
       <c r="H56" s="6">
         <v>3.23</v>
       </c>
-      <c r="I56" s="10">
+      <c r="I56" s="6">
         <v>18.399999999999999</v>
       </c>
     </row>
@@ -3006,7 +3009,7 @@
       <c r="H57" s="6">
         <v>3.3</v>
       </c>
-      <c r="I57" s="10">
+      <c r="I57" s="6">
         <v>21.6</v>
       </c>
     </row>
@@ -3412,6 +3415,9 @@
       <c r="H71" s="6">
         <v>38.4</v>
       </c>
+      <c r="I71" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="72" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A72" s="3" t="s">
@@ -3438,6 +3444,9 @@
       <c r="H72" s="6">
         <v>13.1</v>
       </c>
+      <c r="I72" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="73" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="3" t="s">
@@ -3464,6 +3473,9 @@
       <c r="H73" s="6">
         <v>126.8</v>
       </c>
+      <c r="I73" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="74" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="3" t="s">
@@ -3490,6 +3502,9 @@
       <c r="H74" s="6">
         <v>48</v>
       </c>
+      <c r="I74" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="75" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="3" t="s">
@@ -3516,6 +3531,9 @@
       <c r="H75" s="6">
         <v>142.1</v>
       </c>
+      <c r="I75" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="76" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="3" t="s">
@@ -3542,6 +3560,9 @@
       <c r="H76" s="6">
         <v>59.3</v>
       </c>
+      <c r="I76" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="77" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="3" t="s">
@@ -3568,6 +3589,9 @@
       <c r="H77" s="6">
         <v>243</v>
       </c>
+      <c r="I77" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="78" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="3" t="s">
@@ -3594,6 +3618,9 @@
       <c r="H78" s="6">
         <v>83</v>
       </c>
+      <c r="I78" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="79" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="3" t="s">
@@ -3620,6 +3647,9 @@
       <c r="H79" s="8">
         <v>4.7</v>
       </c>
+      <c r="I79" s="9">
+        <v>20</v>
+      </c>
     </row>
     <row r="80" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="3" t="s">
@@ -3646,8 +3676,11 @@
       <c r="H80" s="5">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I80" s="10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="3" t="s">
         <v>78</v>
       </c>
@@ -3672,8 +3705,11 @@
       <c r="H81" s="5">
         <v>15</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I81" s="10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="3" t="s">
         <v>79</v>
       </c>
@@ -3698,8 +3734,11 @@
       <c r="H82" s="6">
         <v>22.4</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I82" s="11">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" s="3" t="s">
         <v>80</v>
       </c>
@@ -3724,8 +3763,11 @@
       <c r="H83" s="5">
         <v>30</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I83" s="11">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="3" t="s">
         <v>81</v>
       </c>
@@ -3750,8 +3792,11 @@
       <c r="H84" s="7">
         <v>41.5</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I84" s="11">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="3" t="s">
         <v>105</v>
       </c>
@@ -3776,8 +3821,11 @@
       <c r="H85" s="7">
         <v>73</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I85" s="11">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="3" t="s">
         <v>82</v>
       </c>
@@ -3802,8 +3850,11 @@
       <c r="H86" s="7">
         <v>107</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I86" s="11">
+        <v>71.5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="3" t="s">
         <v>83</v>
       </c>
@@ -3828,8 +3879,11 @@
       <c r="H87" s="7">
         <v>154</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I87" s="11">
+        <v>96.8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="3" t="s">
         <v>84</v>
       </c>
@@ -3854,8 +3908,11 @@
       <c r="H88" s="7">
         <v>270</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I88" s="11">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" s="3" t="s">
         <v>85</v>
       </c>
@@ -3880,8 +3937,11 @@
       <c r="H89" s="7">
         <v>442</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I89" s="11">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A90" s="3" t="s">
         <v>86</v>
       </c>
@@ -3906,8 +3966,11 @@
       <c r="H90" s="7">
         <v>657</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I90" s="11">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" s="3" t="s">
         <v>87</v>
       </c>
@@ -3932,8 +3995,11 @@
       <c r="H91" s="7">
         <v>1070</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I91" s="11">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A92" s="3" t="s">
         <v>88</v>
       </c>
@@ -3958,8 +4024,11 @@
       <c r="H92" s="7">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I92" s="11">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="3" t="s">
         <v>89</v>
       </c>
@@ -3984,8 +4053,11 @@
       <c r="H93" s="7">
         <v>3.94</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I93" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="3" t="s">
         <v>90</v>
       </c>
@@ -4010,8 +4082,11 @@
       <c r="H94" s="7">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I94" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="3" t="s">
         <v>91</v>
       </c>
@@ -4036,8 +4111,11 @@
       <c r="H95" s="7">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I95" s="11">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" s="3" t="s">
         <v>123</v>
       </c>
@@ -4062,8 +4140,11 @@
       <c r="H96" s="7">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I96" s="11">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="3" t="s">
         <v>107</v>
       </c>
@@ -4088,8 +4169,11 @@
       <c r="H97" s="7">
         <v>4.2</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I97" s="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="3" t="s">
         <v>108</v>
       </c>
@@ -4114,8 +4198,11 @@
       <c r="H98" s="7">
         <v>8.4</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I98" s="11">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="3" t="s">
         <v>109</v>
       </c>
@@ -4140,8 +4227,11 @@
       <c r="H99" s="7">
         <v>16</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I99" s="11">
+        <v>35.6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" s="3" t="s">
         <v>110</v>
       </c>
@@ -4166,8 +4256,11 @@
       <c r="H100" s="7">
         <v>23.4</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I100" s="11">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="3" t="s">
         <v>111</v>
       </c>
@@ -4192,8 +4285,11 @@
       <c r="H101" s="7">
         <v>32</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I101" s="11">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="3" t="s">
         <v>112</v>
       </c>
@@ -4218,8 +4314,11 @@
       <c r="H102" s="7">
         <v>48</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I102" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" s="3" t="s">
         <v>113</v>
       </c>
@@ -4244,8 +4343,11 @@
       <c r="H103" s="7">
         <v>63</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I103" s="11">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="3" t="s">
         <v>92</v>
       </c>
@@ -4270,8 +4372,11 @@
       <c r="H104" s="7">
         <v>104.2</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I104" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="3" t="s">
         <v>93</v>
       </c>
@@ -4296,8 +4401,11 @@
       <c r="H105" s="7">
         <v>139.6</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I105" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="3" t="s">
         <v>94</v>
       </c>
@@ -4322,8 +4430,11 @@
       <c r="H106" s="7">
         <v>33.6</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I106" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A107" s="3" t="s">
         <v>95</v>
       </c>
@@ -4348,8 +4459,11 @@
       <c r="H107" s="7">
         <v>47.2</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I107" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A108" s="3" t="s">
         <v>96</v>
       </c>
@@ -4374,8 +4488,11 @@
       <c r="H108" s="7">
         <v>84.5</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I108" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A109" s="3" t="s">
         <v>97</v>
       </c>
@@ -4400,8 +4517,11 @@
       <c r="H109" s="7">
         <v>33</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I109" s="12">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A110" s="3" t="s">
         <v>98</v>
       </c>
@@ -4426,8 +4546,11 @@
       <c r="H110" s="7">
         <v>47</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I110" s="12">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A111" s="3" t="s">
         <v>99</v>
       </c>
@@ -4452,8 +4575,11 @@
       <c r="H111" s="7">
         <v>47</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I111" s="12">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="3" t="s">
         <v>100</v>
       </c>
@@ -4478,8 +4604,11 @@
       <c r="H112" s="7">
         <v>104</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I112" s="11">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A113" s="3" t="s">
         <v>101</v>
       </c>
@@ -4504,8 +4633,11 @@
       <c r="H113" s="7">
         <v>158</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I113" s="11">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A114" s="3" t="s">
         <v>102</v>
       </c>
@@ -4530,8 +4662,11 @@
       <c r="H114" s="7">
         <v>309</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I114" s="11">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A115" s="3" t="s">
         <v>103</v>
       </c>
@@ -4556,12 +4691,15 @@
       <c r="H115" s="7">
         <v>340</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="I115" s="11">
+        <v>100.5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
     </row>
-    <row r="117" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added picture display capability
</commit_message>
<xml_diff>
--- a/Cores-Info-Database.xlsx
+++ b/Cores-Info-Database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19725\Desktop\education\college\extracurriculars\pemg research\PEMG_Design_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9AC8855-9782-4822-9E55-ADC660530542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D5C3B5-FA24-4D50-8094-6FDB77EE7BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{FD5E7F2C-425F-4B8A-9B1F-7669120DD1D5}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="164">
   <si>
     <t>E 5</t>
   </si>
@@ -398,6 +398,120 @@
   </si>
   <si>
     <t>Not Available</t>
+  </si>
+  <si>
+    <t>Image Path</t>
+  </si>
+  <si>
+    <t>images/e5.png</t>
+  </si>
+  <si>
+    <t>images/e63.png</t>
+  </si>
+  <si>
+    <t>images/e88.png</t>
+  </si>
+  <si>
+    <t>images/e10555.png</t>
+  </si>
+  <si>
+    <t>images/e136537.png</t>
+  </si>
+  <si>
+    <t>images/e1374.png</t>
+  </si>
+  <si>
+    <t>images/e1484.png</t>
+  </si>
+  <si>
+    <t>images/e1665.png</t>
+  </si>
+  <si>
+    <t>images/e1675.png</t>
+  </si>
+  <si>
+    <t>images/e1685.png</t>
+  </si>
+  <si>
+    <t>images/e1985.png</t>
+  </si>
+  <si>
+    <t>images/e2096.png</t>
+  </si>
+  <si>
+    <t>images/e20106.png</t>
+  </si>
+  <si>
+    <t>images/e201011.png</t>
+  </si>
+  <si>
+    <t>images/e2195.png</t>
+  </si>
+  <si>
+    <t>images/e22156.png</t>
+  </si>
+  <si>
+    <t>images/e25137.png</t>
+  </si>
+  <si>
+    <t>images/e281011.png</t>
+  </si>
+  <si>
+    <t>images/e30157.png</t>
+  </si>
+  <si>
+    <t>images/e321611.png</t>
+  </si>
+  <si>
+    <t>images/e34149.png</t>
+  </si>
+  <si>
+    <t>images/e361811.png</t>
+  </si>
+  <si>
+    <t>images/e401612.png</t>
+  </si>
+  <si>
+    <t>images/e422115.png</t>
+  </si>
+  <si>
+    <t>images/e422120.png</t>
+  </si>
+  <si>
+    <t>images/e472016.png</t>
+  </si>
+  <si>
+    <t>images/e552825.png</t>
+  </si>
+  <si>
+    <t>images/e562419.png</t>
+  </si>
+  <si>
+    <t>images/e653227.png</t>
+  </si>
+  <si>
+    <t>images/e703332.png</t>
+  </si>
+  <si>
+    <t>images/e803820.png</t>
+  </si>
+  <si>
+    <t>images/e1006028.png</t>
+  </si>
+  <si>
+    <t>images/efd1053.png</t>
+  </si>
+  <si>
+    <t>images/efd1585.png</t>
+  </si>
+  <si>
+    <t>images/efd20107.png</t>
+  </si>
+  <si>
+    <t>images/efd25139.png</t>
+  </si>
+  <si>
+    <t>images/efd30159.png</t>
   </si>
 </sst>
 </file>
@@ -928,7 +1042,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -954,16 +1068,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1341,10 +1446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50AB67D-9472-4E0F-AB22-86EA84CCBB8E}">
-  <dimension ref="A1:I117"/>
+  <dimension ref="A1:J117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I116" sqref="I116"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J50" sqref="J50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1358,9 +1463,10 @@
     <col min="7" max="7" width="16.7265625" customWidth="1"/>
     <col min="8" max="8" width="20.7265625" customWidth="1"/>
     <col min="9" max="9" width="16.08984375" customWidth="1"/>
+    <col min="10" max="10" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>104</v>
       </c>
@@ -1388,8 +1494,11 @@
       <c r="I1" s="2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J1" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1417,8 +1526,11 @@
       <c r="I2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1446,8 +1558,11 @@
       <c r="I3" s="7">
         <v>12.8</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1475,8 +1590,11 @@
       <c r="I4" s="7">
         <v>14.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -1504,8 +1622,11 @@
       <c r="I5" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1533,8 +1654,11 @@
       <c r="I6" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -1562,8 +1686,11 @@
       <c r="I7" s="6">
         <v>11.6</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
@@ -1591,8 +1718,11 @@
       <c r="I8" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
@@ -1620,8 +1750,11 @@
       <c r="I9" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1649,8 +1782,11 @@
       <c r="I10" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1678,8 +1814,11 @@
       <c r="I11" s="6">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -1707,8 +1846,11 @@
       <c r="I12" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1736,8 +1878,11 @@
       <c r="I13" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -1765,8 +1910,11 @@
       <c r="I14" s="6">
         <v>41.2</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
@@ -1794,8 +1942,11 @@
       <c r="I15" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J15" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
@@ -1823,8 +1974,11 @@
       <c r="I16" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -1852,8 +2006,11 @@
       <c r="I17" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -1881,8 +2038,11 @@
       <c r="I18" s="6">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
         <v>17</v>
       </c>
@@ -1910,8 +2070,11 @@
       <c r="I19" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
@@ -1939,8 +2102,11 @@
       <c r="I20" s="6">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J20" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
         <v>19</v>
       </c>
@@ -1968,8 +2134,11 @@
       <c r="I21" s="6">
         <v>92.6</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J21" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>20</v>
       </c>
@@ -1997,8 +2166,11 @@
       <c r="I22" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J22" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
@@ -2026,8 +2198,11 @@
       <c r="I23" s="6">
         <v>76.400000000000006</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J23" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>22</v>
       </c>
@@ -2055,8 +2230,11 @@
       <c r="I24" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J24" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
         <v>23</v>
       </c>
@@ -2084,8 +2262,11 @@
       <c r="I25" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J25" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
@@ -2113,8 +2294,11 @@
       <c r="I26" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
@@ -2142,8 +2326,11 @@
       <c r="I27" s="6">
         <v>100</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J27" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
         <v>26</v>
       </c>
@@ -2171,8 +2358,11 @@
       <c r="I28" s="6">
         <v>100</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J28" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
         <v>27</v>
       </c>
@@ -2200,8 +2390,11 @@
       <c r="I29" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>28</v>
       </c>
@@ -2229,8 +2422,11 @@
       <c r="I30" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="3" t="s">
         <v>29</v>
       </c>
@@ -2258,8 +2454,11 @@
       <c r="I31" s="6">
         <v>113</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J31" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>30</v>
       </c>
@@ -2287,8 +2486,11 @@
       <c r="I32" s="6">
         <v>140</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J32" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
         <v>31</v>
       </c>
@@ -2316,8 +2518,11 @@
       <c r="I33" s="6">
         <v>140</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J33" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="3" t="s">
         <v>32</v>
       </c>
@@ -2345,8 +2550,11 @@
       <c r="I34" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J34" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
         <v>33</v>
       </c>
@@ -2374,8 +2582,11 @@
       <c r="I35" s="6">
         <v>246</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J35" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="3" t="s">
         <v>34</v>
       </c>
@@ -2403,8 +2614,11 @@
       <c r="I36" s="6">
         <v>246</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J36" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
         <v>35</v>
       </c>
@@ -2432,8 +2646,11 @@
       <c r="I37" s="6">
         <v>230.5</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J37" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
@@ -2461,8 +2678,11 @@
       <c r="I38" s="6">
         <v>230.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J38" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="3" t="s">
         <v>37</v>
       </c>
@@ -2490,8 +2710,11 @@
       <c r="I39" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J39" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="3" t="s">
         <v>38</v>
       </c>
@@ -2519,8 +2742,11 @@
       <c r="I40" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J40" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="3" t="s">
         <v>39</v>
       </c>
@@ -2548,8 +2774,11 @@
       <c r="I41" s="6">
         <v>342</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J41" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="3" t="s">
         <v>40</v>
       </c>
@@ -2577,8 +2806,11 @@
       <c r="I42" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J42" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="3" t="s">
         <v>41</v>
       </c>
@@ -2606,8 +2838,11 @@
       <c r="I43" s="8">
         <v>35.9</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J43" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="3" t="s">
         <v>42</v>
       </c>
@@ -2635,8 +2870,11 @@
       <c r="I44" s="8">
         <v>40.200000000000003</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J44" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="3" t="s">
         <v>43</v>
       </c>
@@ -2664,8 +2902,11 @@
       <c r="I45" s="8">
         <v>50</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J45" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="3" t="s">
         <v>44</v>
       </c>
@@ -2693,8 +2934,11 @@
       <c r="I46" s="8">
         <v>56.7</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J46" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="3" t="s">
         <v>45</v>
       </c>
@@ -2723,7 +2967,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="3" t="s">
         <v>46</v>
       </c>
@@ -3647,7 +3891,7 @@
       <c r="H79" s="8">
         <v>4.7</v>
       </c>
-      <c r="I79" s="9">
+      <c r="I79" s="8">
         <v>20</v>
       </c>
     </row>
@@ -3676,7 +3920,7 @@
       <c r="H80" s="5">
         <v>9.5</v>
       </c>
-      <c r="I80" s="10">
+      <c r="I80" s="5">
         <v>25</v>
       </c>
     </row>
@@ -3705,7 +3949,7 @@
       <c r="H81" s="5">
         <v>15</v>
       </c>
-      <c r="I81" s="10">
+      <c r="I81" s="5">
         <v>30</v>
       </c>
     </row>
@@ -3734,7 +3978,7 @@
       <c r="H82" s="6">
         <v>22.4</v>
       </c>
-      <c r="I82" s="11">
+      <c r="I82" s="6">
         <v>36</v>
       </c>
     </row>
@@ -3763,7 +4007,7 @@
       <c r="H83" s="5">
         <v>30</v>
       </c>
-      <c r="I83" s="11">
+      <c r="I83" s="6">
         <v>42</v>
       </c>
     </row>
@@ -3792,7 +4036,7 @@
       <c r="H84" s="7">
         <v>41.5</v>
       </c>
-      <c r="I84" s="11">
+      <c r="I84" s="6">
         <v>52</v>
       </c>
     </row>
@@ -3821,7 +4065,7 @@
       <c r="H85" s="7">
         <v>73</v>
       </c>
-      <c r="I85" s="11">
+      <c r="I85" s="6">
         <v>61</v>
       </c>
     </row>
@@ -3850,7 +4094,7 @@
       <c r="H86" s="7">
         <v>107</v>
       </c>
-      <c r="I86" s="11">
+      <c r="I86" s="6">
         <v>71.5</v>
       </c>
     </row>
@@ -3879,7 +4123,7 @@
       <c r="H87" s="7">
         <v>154</v>
       </c>
-      <c r="I87" s="11">
+      <c r="I87" s="6">
         <v>96.8</v>
       </c>
     </row>
@@ -3908,7 +4152,7 @@
       <c r="H88" s="7">
         <v>270</v>
       </c>
-      <c r="I88" s="11">
+      <c r="I88" s="6">
         <v>120</v>
       </c>
     </row>
@@ -3937,7 +4181,7 @@
       <c r="H89" s="7">
         <v>442</v>
       </c>
-      <c r="I89" s="11">
+      <c r="I89" s="6">
         <v>140</v>
       </c>
     </row>
@@ -3966,7 +4210,7 @@
       <c r="H90" s="7">
         <v>657</v>
       </c>
-      <c r="I90" s="11">
+      <c r="I90" s="6">
         <v>158</v>
       </c>
     </row>
@@ -3995,7 +4239,7 @@
       <c r="H91" s="7">
         <v>1070</v>
       </c>
-      <c r="I91" s="11">
+      <c r="I91" s="6">
         <v>210</v>
       </c>
     </row>
@@ -4024,7 +4268,7 @@
       <c r="H92" s="7">
         <v>0.65</v>
       </c>
-      <c r="I92" s="11">
+      <c r="I92" s="6">
         <v>5.8</v>
       </c>
     </row>
@@ -4111,7 +4355,7 @@
       <c r="H95" s="7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="I95" s="11">
+      <c r="I95" s="6">
         <v>14.6</v>
       </c>
     </row>
@@ -4140,7 +4384,7 @@
       <c r="H96" s="7">
         <v>3.6</v>
       </c>
-      <c r="I96" s="11">
+      <c r="I96" s="6">
         <v>19.2</v>
       </c>
     </row>
@@ -4169,7 +4413,7 @@
       <c r="H97" s="7">
         <v>4.2</v>
       </c>
-      <c r="I97" s="11">
+      <c r="I97" s="6">
         <v>22</v>
       </c>
     </row>
@@ -4198,7 +4442,7 @@
       <c r="H98" s="7">
         <v>8.4</v>
       </c>
-      <c r="I98" s="11">
+      <c r="I98" s="6">
         <v>28</v>
       </c>
     </row>
@@ -4227,7 +4471,7 @@
       <c r="H99" s="7">
         <v>16</v>
       </c>
-      <c r="I99" s="11">
+      <c r="I99" s="6">
         <v>35.6</v>
       </c>
     </row>
@@ -4256,7 +4500,7 @@
       <c r="H100" s="7">
         <v>23.4</v>
       </c>
-      <c r="I100" s="11">
+      <c r="I100" s="6">
         <v>44</v>
       </c>
     </row>
@@ -4285,7 +4529,7 @@
       <c r="H101" s="7">
         <v>32</v>
       </c>
-      <c r="I101" s="11">
+      <c r="I101" s="6">
         <v>52</v>
       </c>
     </row>
@@ -4314,7 +4558,7 @@
       <c r="H102" s="7">
         <v>48</v>
       </c>
-      <c r="I102" s="11">
+      <c r="I102" s="6">
         <v>60</v>
       </c>
     </row>
@@ -4343,7 +4587,7 @@
       <c r="H103" s="7">
         <v>63</v>
       </c>
-      <c r="I103" s="11">
+      <c r="I103" s="6">
         <v>73</v>
       </c>
     </row>
@@ -4517,7 +4761,7 @@
       <c r="H109" s="7">
         <v>33</v>
       </c>
-      <c r="I109" s="12">
+      <c r="I109" s="7">
         <v>56</v>
       </c>
     </row>
@@ -4546,7 +4790,7 @@
       <c r="H110" s="7">
         <v>47</v>
       </c>
-      <c r="I110" s="12">
+      <c r="I110" s="7">
         <v>56</v>
       </c>
     </row>
@@ -4575,7 +4819,7 @@
       <c r="H111" s="7">
         <v>47</v>
       </c>
-      <c r="I111" s="12">
+      <c r="I111" s="7">
         <v>66</v>
       </c>
     </row>
@@ -4604,7 +4848,7 @@
       <c r="H112" s="7">
         <v>104</v>
       </c>
-      <c r="I112" s="11">
+      <c r="I112" s="6">
         <v>62</v>
       </c>
     </row>
@@ -4633,7 +4877,7 @@
       <c r="H113" s="7">
         <v>158</v>
       </c>
-      <c r="I113" s="11">
+      <c r="I113" s="6">
         <v>76</v>
       </c>
     </row>
@@ -4662,7 +4906,7 @@
       <c r="H114" s="7">
         <v>309</v>
       </c>
-      <c r="I114" s="11">
+      <c r="I114" s="6">
         <v>87</v>
       </c>
     </row>
@@ -4691,7 +4935,7 @@
       <c r="H115" s="7">
         <v>340</v>
       </c>
-      <c r="I115" s="11">
+      <c r="I115" s="6">
         <v>100.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added all the necessary photos
</commit_message>
<xml_diff>
--- a/Cores-Info-Database.xlsx
+++ b/Cores-Info-Database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19725\Desktop\education\college\extracurriculars\pemg research\PEMG_Design_Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D5C3B5-FA24-4D50-8094-6FDB77EE7BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E11FA81-DDFA-45D4-8EC8-5D9077CB6B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{FD5E7F2C-425F-4B8A-9B1F-7669120DD1D5}"/>
   </bookViews>
@@ -16,11 +16,12 @@
     <sheet name="Cores-Info-Database" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="230">
   <si>
     <t>E 5</t>
   </si>
@@ -512,6 +513,204 @@
   </si>
   <si>
     <t>images/efd30159.png</t>
+  </si>
+  <si>
+    <t>images/elp22616.png</t>
+  </si>
+  <si>
+    <t>images/elp32620.png</t>
+  </si>
+  <si>
+    <t>images/elp38825.png</t>
+  </si>
+  <si>
+    <t>images/elp431028.png</t>
+  </si>
+  <si>
+    <t>images/elp641050.png</t>
+  </si>
+  <si>
+    <t>images/elp1022038.png</t>
+  </si>
+  <si>
+    <t>images/er955.png</t>
+  </si>
+  <si>
+    <t>images/er115.png</t>
+  </si>
+  <si>
+    <t>images/er1456.png</t>
+  </si>
+  <si>
+    <t>images/er18310.png</t>
+  </si>
+  <si>
+    <t>images/er23513.png</t>
+  </si>
+  <si>
+    <t>images/er25615.png</t>
+  </si>
+  <si>
+    <t>images/er281711.png</t>
+  </si>
+  <si>
+    <t>images/er32521.png</t>
+  </si>
+  <si>
+    <t>images/elp18410.png</t>
+  </si>
+  <si>
+    <t>images/elp14355.png</t>
+  </si>
+  <si>
+    <t>images/er352011.png</t>
+  </si>
+  <si>
+    <t>images/er422215.png</t>
+  </si>
+  <si>
+    <t>images/er461718.png</t>
+  </si>
+  <si>
+    <t>images/er492717.png</t>
+  </si>
+  <si>
+    <t>images/er541818.png</t>
+  </si>
+  <si>
+    <t>images/eq1328587.png</t>
+  </si>
+  <si>
+    <t>images/i13187.png</t>
+  </si>
+  <si>
+    <t>images/eq206314.png</t>
+  </si>
+  <si>
+    <t>images/i202314.png</t>
+  </si>
+  <si>
+    <t>images/i252318.png</t>
+  </si>
+  <si>
+    <t>images/eq30820.png</t>
+  </si>
+  <si>
+    <t>images/i302720.png</t>
+  </si>
+  <si>
+    <t>images/eq255618.png</t>
+  </si>
+  <si>
+    <t>images/rm4.png</t>
+  </si>
+  <si>
+    <t>images/rm5.png</t>
+  </si>
+  <si>
+    <t>images/rm6.png</t>
+  </si>
+  <si>
+    <t>images/rm7.png</t>
+  </si>
+  <si>
+    <t>images/rm8.png</t>
+  </si>
+  <si>
+    <t>images/rm10.png</t>
+  </si>
+  <si>
+    <t>images/rm12.png</t>
+  </si>
+  <si>
+    <t>images/rm14.png</t>
+  </si>
+  <si>
+    <t>images/pm5039.png</t>
+  </si>
+  <si>
+    <t>images/pm6249.png</t>
+  </si>
+  <si>
+    <t>images/pm7459.png</t>
+  </si>
+  <si>
+    <t>images/pm8770.png</t>
+  </si>
+  <si>
+    <t>images/pm11493.png</t>
+  </si>
+  <si>
+    <t>images/p3326.png</t>
+  </si>
+  <si>
+    <t>images/p4641.png</t>
+  </si>
+  <si>
+    <t>images/p5833.png</t>
+  </si>
+  <si>
+    <t>images/p74.png</t>
+  </si>
+  <si>
+    <t>images/p95.png</t>
+  </si>
+  <si>
+    <t>images/p117.png</t>
+  </si>
+  <si>
+    <t>images/p148.png</t>
+  </si>
+  <si>
+    <t>images/p1811.png</t>
+  </si>
+  <si>
+    <t>images/p2213.png</t>
+  </si>
+  <si>
+    <t>images/p2616.png</t>
+  </si>
+  <si>
+    <t>images/p3019.png</t>
+  </si>
+  <si>
+    <t>images/p3622.png</t>
+  </si>
+  <si>
+    <t>images/p4125.png</t>
+  </si>
+  <si>
+    <t>images/p4728.png</t>
+  </si>
+  <si>
+    <t>images/p16116.png</t>
+  </si>
+  <si>
+    <t>images/p2016.png</t>
+  </si>
+  <si>
+    <t>images/p2020.png</t>
+  </si>
+  <si>
+    <t>images/p2620.png</t>
+  </si>
+  <si>
+    <t>images/p2625.png</t>
+  </si>
+  <si>
+    <t>images/p3220.png</t>
+  </si>
+  <si>
+    <t>images/p3230.png</t>
+  </si>
+  <si>
+    <t>images/p3535.png</t>
+  </si>
+  <si>
+    <t>images/p4040.png</t>
+  </si>
+  <si>
+    <t>images/p5050.png</t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1241,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1067,9 +1266,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1448,8 +1644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50AB67D-9472-4E0F-AB22-86EA84CCBB8E}">
   <dimension ref="A1:J117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K114" sqref="K114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1466,7 +1662,7 @@
     <col min="10" max="10" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>104</v>
       </c>
@@ -1494,7 +1690,7 @@
       <c r="I1" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="5" t="s">
         <v>126</v>
       </c>
     </row>
@@ -2966,6 +3162,9 @@
       <c r="I47" t="s">
         <v>125</v>
       </c>
+      <c r="J47" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="48" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="3" t="s">
@@ -2995,8 +3194,11 @@
       <c r="I48" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J48" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="3" t="s">
         <v>47</v>
       </c>
@@ -3024,8 +3226,11 @@
       <c r="I49" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J49" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="3" t="s">
         <v>48</v>
       </c>
@@ -3053,8 +3258,11 @@
       <c r="I50" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J50" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="3" t="s">
         <v>49</v>
       </c>
@@ -3082,8 +3290,11 @@
       <c r="I51" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J51" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="3" t="s">
         <v>50</v>
       </c>
@@ -3111,8 +3322,11 @@
       <c r="I52" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J52" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="3" t="s">
         <v>51</v>
       </c>
@@ -3140,8 +3354,11 @@
       <c r="I53" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J53" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="3" t="s">
         <v>52</v>
       </c>
@@ -3169,8 +3386,11 @@
       <c r="I54" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J54" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="3" t="s">
         <v>53</v>
       </c>
@@ -3198,8 +3418,11 @@
       <c r="I55" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J55" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="3" t="s">
         <v>54</v>
       </c>
@@ -3227,8 +3450,11 @@
       <c r="I56" s="6">
         <v>18.399999999999999</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J56" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="3" t="s">
         <v>55</v>
       </c>
@@ -3256,8 +3482,11 @@
       <c r="I57" s="6">
         <v>21.6</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J57" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="3" t="s">
         <v>56</v>
       </c>
@@ -3285,8 +3514,11 @@
       <c r="I58" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J58" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="3" t="s">
         <v>57</v>
       </c>
@@ -3314,8 +3546,11 @@
       <c r="I59" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J59" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="3" t="s">
         <v>58</v>
       </c>
@@ -3343,8 +3578,11 @@
       <c r="I60" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J60" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="3" t="s">
         <v>59</v>
       </c>
@@ -3372,8 +3610,11 @@
       <c r="I61" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J61" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="3" t="s">
         <v>60</v>
       </c>
@@ -3401,8 +3642,11 @@
       <c r="I62" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J62" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="3" t="s">
         <v>61</v>
       </c>
@@ -3430,8 +3674,11 @@
       <c r="I63" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J63" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="3" t="s">
         <v>62</v>
       </c>
@@ -3459,8 +3706,11 @@
       <c r="I64" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J64" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="3" t="s">
         <v>63</v>
       </c>
@@ -3488,8 +3738,11 @@
       <c r="I65" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J65" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="3" t="s">
         <v>64</v>
       </c>
@@ -3517,8 +3770,11 @@
       <c r="I66" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J66" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" s="3" t="s">
         <v>65</v>
       </c>
@@ -3546,8 +3802,11 @@
       <c r="I67" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J67" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="3" t="s">
         <v>66</v>
       </c>
@@ -3575,8 +3834,11 @@
       <c r="I68" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J68" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="3" t="s">
         <v>67</v>
       </c>
@@ -3604,8 +3866,11 @@
       <c r="I69" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J69" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="3" t="s">
         <v>68</v>
       </c>
@@ -3633,8 +3898,11 @@
       <c r="I70" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J70" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="3" t="s">
         <v>69</v>
       </c>
@@ -3662,8 +3930,11 @@
       <c r="I71" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J71" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A72" s="3" t="s">
         <v>70</v>
       </c>
@@ -3691,8 +3962,11 @@
       <c r="I72" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J72" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="3" t="s">
         <v>71</v>
       </c>
@@ -3720,8 +3994,11 @@
       <c r="I73" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J73" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="3" t="s">
         <v>72</v>
       </c>
@@ -3749,8 +4026,11 @@
       <c r="I74" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J74" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="3" t="s">
         <v>73</v>
       </c>
@@ -3778,8 +4058,11 @@
       <c r="I75" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J75" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="3" t="s">
         <v>74</v>
       </c>
@@ -3807,8 +4090,11 @@
       <c r="I76" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J76" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="3" t="s">
         <v>75</v>
       </c>
@@ -3836,8 +4122,11 @@
       <c r="I77" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J77" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="3" t="s">
         <v>76</v>
       </c>
@@ -3865,8 +4154,11 @@
       <c r="I78" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J78" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="3" t="s">
         <v>77</v>
       </c>
@@ -3894,8 +4186,11 @@
       <c r="I79" s="8">
         <v>20</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J79" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="3" t="s">
         <v>106</v>
       </c>
@@ -3923,8 +4218,11 @@
       <c r="I80" s="5">
         <v>25</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J80" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="3" t="s">
         <v>78</v>
       </c>
@@ -3952,8 +4250,11 @@
       <c r="I81" s="5">
         <v>30</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J81" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="3" t="s">
         <v>79</v>
       </c>
@@ -3981,8 +4282,11 @@
       <c r="I82" s="6">
         <v>36</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J82" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" s="3" t="s">
         <v>80</v>
       </c>
@@ -4010,8 +4314,11 @@
       <c r="I83" s="6">
         <v>42</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J83" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="3" t="s">
         <v>81</v>
       </c>
@@ -4039,8 +4346,11 @@
       <c r="I84" s="6">
         <v>52</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J84" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="3" t="s">
         <v>105</v>
       </c>
@@ -4068,8 +4378,11 @@
       <c r="I85" s="6">
         <v>61</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J85" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="3" t="s">
         <v>82</v>
       </c>
@@ -4097,8 +4410,11 @@
       <c r="I86" s="6">
         <v>71.5</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J86" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="3" t="s">
         <v>83</v>
       </c>
@@ -4126,8 +4442,11 @@
       <c r="I87" s="6">
         <v>96.8</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J87" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="3" t="s">
         <v>84</v>
       </c>
@@ -4155,8 +4474,11 @@
       <c r="I88" s="6">
         <v>120</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J88" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" s="3" t="s">
         <v>85</v>
       </c>
@@ -4184,8 +4506,11 @@
       <c r="I89" s="6">
         <v>140</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J89" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A90" s="3" t="s">
         <v>86</v>
       </c>
@@ -4213,8 +4538,11 @@
       <c r="I90" s="6">
         <v>158</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J90" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" s="3" t="s">
         <v>87</v>
       </c>
@@ -4242,8 +4570,11 @@
       <c r="I91" s="6">
         <v>210</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J91" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A92" s="3" t="s">
         <v>88</v>
       </c>
@@ -4271,8 +4602,11 @@
       <c r="I92" s="6">
         <v>5.8</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J92" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A93" s="3" t="s">
         <v>89</v>
       </c>
@@ -4300,8 +4634,11 @@
       <c r="I93" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J93" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="3" t="s">
         <v>90</v>
       </c>
@@ -4329,8 +4666,11 @@
       <c r="I94" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J94" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="3" t="s">
         <v>91</v>
       </c>
@@ -4358,8 +4698,11 @@
       <c r="I95" s="6">
         <v>14.6</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J95" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" s="3" t="s">
         <v>123</v>
       </c>
@@ -4387,8 +4730,11 @@
       <c r="I96" s="6">
         <v>19.2</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J96" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="3" t="s">
         <v>107</v>
       </c>
@@ -4416,8 +4762,11 @@
       <c r="I97" s="6">
         <v>22</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J97" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="3" t="s">
         <v>108</v>
       </c>
@@ -4445,8 +4794,11 @@
       <c r="I98" s="6">
         <v>28</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J98" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="3" t="s">
         <v>109</v>
       </c>
@@ -4474,8 +4826,11 @@
       <c r="I99" s="6">
         <v>35.6</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J99" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" s="3" t="s">
         <v>110</v>
       </c>
@@ -4503,8 +4858,11 @@
       <c r="I100" s="6">
         <v>44</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J100" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="3" t="s">
         <v>111</v>
       </c>
@@ -4532,8 +4890,11 @@
       <c r="I101" s="6">
         <v>52</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J101" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A102" s="3" t="s">
         <v>112</v>
       </c>
@@ -4561,8 +4922,11 @@
       <c r="I102" s="6">
         <v>60</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J102" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A103" s="3" t="s">
         <v>113</v>
       </c>
@@ -4590,8 +4954,11 @@
       <c r="I103" s="6">
         <v>73</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J103" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A104" s="3" t="s">
         <v>92</v>
       </c>
@@ -4619,8 +4986,11 @@
       <c r="I104" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J104" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="3" t="s">
         <v>93</v>
       </c>
@@ -4648,8 +5018,11 @@
       <c r="I105" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J105" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="3" t="s">
         <v>94</v>
       </c>
@@ -4677,8 +5050,11 @@
       <c r="I106" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J106" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A107" s="3" t="s">
         <v>95</v>
       </c>
@@ -4706,8 +5082,11 @@
       <c r="I107" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J107" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A108" s="3" t="s">
         <v>96</v>
       </c>
@@ -4735,8 +5114,11 @@
       <c r="I108" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J108" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A109" s="3" t="s">
         <v>97</v>
       </c>
@@ -4764,8 +5146,11 @@
       <c r="I109" s="7">
         <v>56</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J109" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A110" s="3" t="s">
         <v>98</v>
       </c>
@@ -4793,8 +5178,11 @@
       <c r="I110" s="7">
         <v>56</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J110" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A111" s="3" t="s">
         <v>99</v>
       </c>
@@ -4822,8 +5210,11 @@
       <c r="I111" s="7">
         <v>66</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J111" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A112" s="3" t="s">
         <v>100</v>
       </c>
@@ -4851,8 +5242,11 @@
       <c r="I112" s="6">
         <v>62</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J112" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A113" s="3" t="s">
         <v>101</v>
       </c>
@@ -4880,8 +5274,11 @@
       <c r="I113" s="6">
         <v>76</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J113" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A114" s="3" t="s">
         <v>102</v>
       </c>
@@ -4909,8 +5306,11 @@
       <c r="I114" s="6">
         <v>87</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J114" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A115" s="3" t="s">
         <v>103</v>
       </c>
@@ -4938,12 +5338,15 @@
       <c r="I115" s="6">
         <v>100.5</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="J115" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
     </row>
-    <row r="117" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
     </row>

</xml_diff>